<commit_message>
updated functions list, 7th august 2017
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15192" windowHeight="6180" tabRatio="944" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -17,12 +17,12 @@
     <sheet name="TLM" sheetId="9" r:id="rId8"/>
     <sheet name="exmple files" sheetId="7" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="117">
   <si>
     <t>method</t>
   </si>
@@ -347,13 +347,40 @@
   </si>
   <si>
     <t>update the parameters of the memory, that holds the joint positions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">returns the external torques of the joints, for more information refer to matlab file (getJointsExternalTorques.m) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">returns the measured torques of the joints, for more information refer to matlab file (getJointsMeasuredTorques.m) </t>
+  </si>
+  <si>
+    <t xml:space="preserve">returns the measured torque of the defined joint, for more information refer to matlab file (getMeasuredTorqueAtJoint.m) </t>
+  </si>
+  <si>
+    <t>getEEFOrientationQuat</t>
+  </si>
+  <si>
+    <t>getEEFOrientationR</t>
+  </si>
+  <si>
+    <t>getEEFOrientationEuler</t>
+  </si>
+  <si>
+    <t>returns the orientation of the end effector, it returns the rotation of the endeffector, relative to some defined frame. The returned rotation is expressed by a rotation matrix</t>
+  </si>
+  <si>
+    <t>returns the orientation of the end effector, it returns the rotation of the endeffector, relative to some defined frame. The returned rotation is expressed by a quatrinion</t>
+  </si>
+  <si>
+    <t>returns the orientation of the end effector, it returns the rotation of the endeffector, relative to some defined frame. The returned rotation is expressed by a euler angles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -366,6 +393,13 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -587,7 +621,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -633,14 +667,14 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -651,6 +685,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1039,7 +1083,7 @@
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1348,10 +1392,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C15"/>
+  <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1380,6 +1424,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
@@ -1391,6 +1436,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
+        <f t="shared" ref="A4:A18" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
@@ -1402,100 +1448,110 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" t="s">
-        <v>27</v>
+      <c r="B5" s="26" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>29</v>
+      <c r="B6" s="26" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
-        <v>30</v>
+      <c r="B7" s="26" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
+        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>31</v>
+        <v>24</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
+        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>34</v>
+        <v>30</v>
+      </c>
+      <c r="C10" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>40</v>
+        <v>109</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
+        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="C12" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
+        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>110</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" t="s">
         <v>40</v>
@@ -1503,488 +1559,753 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C15" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>37</v>
+      </c>
+      <c r="C16" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>38</v>
+      </c>
+      <c r="C17" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" t="s">
+        <v>40</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C52"/>
+  <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="C40" sqref="C38:C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.88671875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="33.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="59.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="59.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B1" s="2" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C1" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="17" t="s">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="19"/>
-    </row>
-    <row r="4" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="25"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="C5" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="D6" s="8" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" s="9"/>
-      <c r="B7" s="3" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <f>A6+1</f>
+        <v>2</v>
+      </c>
+      <c r="B7" s="9"/>
+      <c r="C7" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="D7" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="27" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="7" t="s">
+    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <f t="shared" ref="A8:A55" si="0">A7+1</f>
+        <v>3</v>
+      </c>
+      <c r="B8" s="7" t="s">
         <v>75</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="D8" s="8" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="9"/>
-      <c r="B9" s="3" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B9" s="9"/>
+      <c r="C9" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="D9" s="8" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="9"/>
-      <c r="B10" s="3" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B10" s="9"/>
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="D10" s="8" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="7" t="s">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B11" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="8" t="s">
+      <c r="D11" s="8" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" s="9"/>
-      <c r="B12" s="3" t="s">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B12" s="9"/>
+      <c r="C12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="D12" s="8" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" s="9"/>
-      <c r="B13" s="3" t="s">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" s="9"/>
-      <c r="B14" s="3" t="s">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B14" s="9"/>
+      <c r="C14" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="D14" s="8" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="9"/>
-      <c r="B15" s="3" t="s">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B15" s="9"/>
+      <c r="C15" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="D15" s="8" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="9"/>
-      <c r="B16" s="3" t="s">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B16" s="9"/>
+      <c r="C16" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="D16" s="8" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="17" spans="1:3" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="13"/>
-      <c r="B17" s="14" t="s">
+    <row r="17" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B17" s="13"/>
+      <c r="C17" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="15" t="s">
+      <c r="D17" s="15" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="18" spans="1:3" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18" s="13"/>
-      <c r="B18" s="14" t="s">
+    <row r="18" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B18" s="13"/>
+      <c r="C18" s="14" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="D18" s="15" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:3" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A19" s="13"/>
-      <c r="B19" s="14" t="s">
+    <row r="19" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B19" s="13"/>
+      <c r="C19" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="D19" s="15" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="20" spans="1:3" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20" s="13"/>
-      <c r="B20" s="14" t="s">
+    <row r="20" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="D20" s="15" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="21" spans="1:3" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14" t="s">
+    <row r="21" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B21" s="13"/>
+      <c r="C21" s="14" t="s">
         <v>101</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="D21" s="15" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22" s="7" t="s">
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B22" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="C22" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="D22" s="8" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23" s="9"/>
-      <c r="B23" s="3" t="s">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="B23" s="9"/>
+      <c r="C23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D23" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24" s="9"/>
-      <c r="B24" s="3" t="s">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B24" s="9"/>
+      <c r="C24" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="C24" s="8" t="s">
+      <c r="D24" s="8" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="9"/>
-      <c r="B25" s="3" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B25" s="9"/>
+      <c r="C25" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="C25" s="8" t="s">
+      <c r="D25" s="8" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="9"/>
-      <c r="B26" s="3" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B26" s="9"/>
+      <c r="C26" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C26" s="8" t="s">
+      <c r="D26" s="8" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="3" t="s">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B27" s="9"/>
+      <c r="C27" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="C27" s="8" t="s">
+      <c r="D27" s="8" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" s="9"/>
-      <c r="B28" s="3" t="s">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B28" s="9"/>
+      <c r="C28" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C28" s="8" t="s">
+      <c r="D28" s="8" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" s="9"/>
-      <c r="B29" s="3" t="s">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="9"/>
+      <c r="C29" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="C29" s="8" t="s">
+      <c r="D29" s="8" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" s="9"/>
-      <c r="B30" s="3" t="s">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="D30" s="8" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A31" s="9"/>
-      <c r="B31" s="3" t="s">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B31" s="9"/>
+      <c r="C31" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C31" s="8" t="s">
+      <c r="D31" s="8" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A32" s="9"/>
-      <c r="B32" s="3" t="s">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B32" s="9"/>
+      <c r="C32" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C32" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A33" s="9"/>
-      <c r="B33" s="3" t="s">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B33" s="9"/>
+      <c r="C33" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C33" s="8" t="s">
+      <c r="D33" s="8" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A34" s="9"/>
-      <c r="B34" s="3" t="s">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B34" s="9"/>
+      <c r="C34" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C34" s="8" t="s">
+      <c r="D34" s="8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A35" s="7" t="s">
+    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B35" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="C35" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C35" s="8" t="s">
+      <c r="D35" s="8" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A36" s="9"/>
-      <c r="B36" s="3" t="s">
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B36" s="9"/>
+      <c r="C36" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="8" t="s">
+      <c r="D36" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37" s="9"/>
-      <c r="B37" s="3" t="s">
+    <row r="37" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B37" s="9"/>
+      <c r="C37" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="C37" s="8" t="s">
+      <c r="D37" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="9"/>
-      <c r="B38" s="3" t="s">
+    <row r="38" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B38" s="17"/>
+      <c r="C38" s="18" t="s">
+        <v>112</v>
+      </c>
+      <c r="D38" s="19" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B39" s="17"/>
+      <c r="C39" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="D39" s="19" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B40" s="17"/>
+      <c r="C40" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B41" s="9"/>
+      <c r="C41" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C38" s="8" t="s">
+      <c r="D41" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39" s="9"/>
-      <c r="B39" s="3" t="s">
+    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B42" s="9"/>
+      <c r="C42" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C39" s="8" t="s">
+      <c r="D42" s="8" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A40" s="9"/>
-      <c r="B40" s="3" t="s">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B43" s="9"/>
+      <c r="C43" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C40" s="8"/>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A41" s="9"/>
-      <c r="B41" s="3" t="s">
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B44" s="9"/>
+      <c r="C44" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C41" s="8"/>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A42" s="9"/>
-      <c r="B42" s="3" t="s">
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B45" s="9"/>
+      <c r="C45" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C42" s="8" t="s">
+      <c r="D45" s="8" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A43" s="9"/>
-      <c r="B43" s="3" t="s">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B46" s="9"/>
+      <c r="C46" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C43" s="8"/>
-    </row>
-    <row r="44" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A44" s="9"/>
-      <c r="B44" s="3" t="s">
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B47" s="9"/>
+      <c r="C47" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C44" s="8" t="s">
+      <c r="D47" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A45" s="9"/>
-      <c r="B45" s="3" t="s">
+    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B48" s="9"/>
+      <c r="C48" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C45" s="8" t="s">
+      <c r="D48" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
-      <c r="B46" s="3" t="s">
+    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B49" s="9"/>
+      <c r="C49" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="D49" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A47" s="9"/>
-      <c r="B47" s="3" t="s">
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B50" s="9"/>
+      <c r="C50" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C47" s="8" t="s">
+      <c r="D50" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A48" s="9"/>
-      <c r="B48" s="3" t="s">
+    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B51" s="9"/>
+      <c r="C51" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C48" s="8" t="s">
+      <c r="D51" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A49" s="9"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="8"/>
-    </row>
-    <row r="50" spans="1:3" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A50" s="7" t="s">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B52" s="9"/>
+      <c r="C52" s="3"/>
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B53" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C53" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="C50" s="8" t="s">
+      <c r="D53" s="8" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A51" s="9"/>
-      <c r="B51" s="3" t="s">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B54" s="9"/>
+      <c r="C54" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C51" s="8" t="s">
+      <c r="D54" s="8" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="10"/>
-      <c r="B52" s="11" t="s">
+    <row r="55" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B55" s="10"/>
+      <c r="C55" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="D55" s="12" t="s">
         <v>86</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A3:C3"/>
+    <mergeCell ref="B3:D3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
More illustrations about the robot functionalities are added
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" activeTab="6"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15220" windowHeight="6230" tabRatio="944" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -16,13 +16,14 @@
     <sheet name="read parameters" sheetId="4" r:id="rId7"/>
     <sheet name="TLM" sheetId="9" r:id="rId8"/>
     <sheet name="exmple files" sheetId="7" r:id="rId9"/>
+    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="137">
   <si>
     <t>method</t>
   </si>
@@ -205,21 +206,6 @@
   </si>
   <si>
     <t>sets the output of Pin2 to low level.</t>
-  </si>
-  <si>
-    <t>kuka0_do_some_stuff</t>
-  </si>
-  <si>
-    <t>kuka0_longTest</t>
-  </si>
-  <si>
-    <t>kuka0_move_lin</t>
-  </si>
-  <si>
-    <t>kuka0_move_ptp</t>
-  </si>
-  <si>
-    <t>The robot moves</t>
   </si>
   <si>
     <t>movePTPHomeJointSpace</t>
@@ -374,6 +360,81 @@
   </si>
   <si>
     <t>returns the orientation of the end effector, it returns the rotation of the endeffector, relative to some defined frame. The returned rotation is expressed by a euler angles</t>
+  </si>
+  <si>
+    <t>with the KST for realtime control of the manipulator.</t>
+  </si>
+  <si>
+    <t>In this example the iiwa robot is controlled in realtime</t>
+  </si>
+  <si>
+    <t>using a gamepad controller, the example is in the folder</t>
+  </si>
+  <si>
+    <t>(realtimeControlOfJointSpaceUsingGamePad) of the github</t>
+  </si>
+  <si>
+    <t>repository.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_circles: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_directServo: </t>
+  </si>
+  <si>
+    <t>real-time control of the robot joints from remote PC.</t>
+  </si>
+  <si>
+    <t>in this example the manipulator perform circular motions</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_do_some_stuff: </t>
+  </si>
+  <si>
+    <t>demonstrates how to use the some of the Toolbox functionalities</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_getters: </t>
+  </si>
+  <si>
+    <t>how to acquire data from robot</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_longTest: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_move_lin: </t>
+  </si>
+  <si>
+    <t>move robot in linear motions, using remote PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_move_lin_relative: </t>
+  </si>
+  <si>
+    <t xml:space="preserve">move robot in linear motion </t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_move_ptp: </t>
+  </si>
+  <si>
+    <t>perform point to point motions using remote PC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_move_sequare: </t>
+  </si>
+  <si>
+    <t>move along a sequare</t>
+  </si>
+  <si>
+    <t xml:space="preserve">kuka0_gampade_jointsPosControl: </t>
+  </si>
+  <si>
+    <t>example of integrating external hardware (gamepad) for real time conotrol of the joints of the robot.</t>
+  </si>
+  <si>
+    <t>long test of the various funcitonalities of the toolbox</t>
   </si>
 </sst>
 </file>
@@ -621,7 +682,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -676,6 +737,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -694,13 +756,86 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -717,10 +852,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="CDE3DE"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1005,21 +1140,21 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="20" t="s">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B2" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1027,6 +1162,20 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
@@ -1038,12 +1187,12 @@
       <selection activeCell="B2" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="3" width="44.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1051,7 +1200,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1062,7 +1211,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1086,12 +1235,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="3" width="44.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1099,7 +1248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1110,7 +1259,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1121,7 +1270,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1132,7 +1281,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1140,7 +1289,7 @@
         <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
     </row>
   </sheetData>
@@ -1156,12 +1305,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="3" width="44.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1169,7 +1318,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1180,7 +1329,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1191,26 +1340,26 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="C4" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -1226,7 +1375,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1240,12 +1389,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="3" width="44.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1253,7 +1402,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1264,7 +1413,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1272,10 +1421,10 @@
         <v>18</v>
       </c>
       <c r="C3" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1286,7 +1435,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1297,7 +1446,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1308,7 +1457,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1319,7 +1468,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1330,7 +1479,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1341,7 +1490,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1352,7 +1501,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1363,7 +1512,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1374,7 +1523,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1394,16 +1543,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="3" width="44.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1411,7 +1560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1422,7 +1571,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1434,7 +1583,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <f t="shared" ref="A4:A18" si="0">A3+1</f>
         <v>3</v>
@@ -1446,34 +1595,34 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="26" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B5" s="20" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="26" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B6" s="20" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="26" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B7" s="20" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1485,7 +1634,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1497,7 +1646,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1506,10 +1655,10 @@
         <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1518,10 +1667,10 @@
         <v>31</v>
       </c>
       <c r="C11" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1533,7 +1682,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1542,10 +1691,10 @@
         <v>34</v>
       </c>
       <c r="C13" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1557,7 +1706,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1569,7 +1718,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1581,7 +1730,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1593,7 +1742,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1619,45 +1768,45 @@
       <selection activeCell="C40" sqref="C38:C40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="59.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.81640625" customWidth="1"/>
+    <col min="2" max="2" width="17.90625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.36328125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="59.90625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C1" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="23" t="s">
-        <v>70</v>
-      </c>
-      <c r="C3" s="24"/>
-      <c r="D3" s="25"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B3" s="24" t="s">
+        <v>65</v>
+      </c>
+      <c r="C3" s="25"/>
+      <c r="D3" s="26"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -1666,7 +1815,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7">
         <f>A6+1</f>
         <v>2</v>
@@ -1679,13 +1828,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <f t="shared" ref="A8:A55" si="0">A7+1</f>
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
@@ -1694,7 +1843,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1707,7 +1856,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1720,13 +1869,13 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>7</v>
@@ -1735,7 +1884,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1748,139 +1897,139 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B13" s="9"/>
       <c r="C13" s="3" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="3" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="3" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="16" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B17" s="13"/>
       <c r="C17" s="14" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B18" s="13"/>
       <c r="C18" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="D18" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D18" s="15" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:4" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="14" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="14" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="D21" s="15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D22" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -1890,23 +2039,23 @@
         <v>18</v>
       </c>
       <c r="D23" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B24" s="9"/>
       <c r="C24" s="3" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -1919,7 +2068,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -1932,7 +2081,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -1945,7 +2094,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -1958,7 +2107,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -1971,7 +2120,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -1984,7 +2133,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -1997,7 +2146,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2010,7 +2159,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2023,7 +2172,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2036,13 +2185,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>20</v>
@@ -2051,7 +2200,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2064,72 +2213,72 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="3" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B38" s="17"/>
       <c r="C38" s="18" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
       <c r="D38" s="19" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B39" s="17"/>
       <c r="C39" s="18" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
       <c r="D39" s="19" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="18" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="D40" s="19" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="3" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="D41" s="8" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2142,7 +2291,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2153,7 +2302,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2164,7 +2313,7 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2177,7 +2326,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2188,7 +2337,7 @@
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2201,7 +2350,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2214,7 +2363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2227,7 +2376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2240,7 +2389,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2253,7 +2402,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2262,45 +2411,45 @@
       <c r="C52" s="3"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>81</v>
+        <v>76</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="3" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="D54" s="8" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B55" s="10"/>
       <c r="C55" s="11" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="D55" s="12" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2314,54 +2463,156 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:D4"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="35.44140625" customWidth="1"/>
-    <col min="4" max="4" width="51.21875" customWidth="1"/>
+    <col min="1" max="1" width="4.453125" customWidth="1"/>
+    <col min="2" max="2" width="35.453125" customWidth="1"/>
+    <col min="3" max="3" width="53.36328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B1">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A1">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B2">
+      <c r="B1" t="s">
+        <v>117</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A2">
         <v>2</v>
       </c>
+      <c r="B2" t="s">
+        <v>118</v>
+      </c>
       <c r="C2" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B3">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A3">
         <v>3</v>
       </c>
+      <c r="B3" t="s">
+        <v>121</v>
+      </c>
       <c r="C3" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.3">
-      <c r="B4">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A4">
         <v>4</v>
       </c>
+      <c r="B4" t="s">
+        <v>123</v>
+      </c>
       <c r="C4" t="s">
-        <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A6">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>126</v>
+      </c>
+      <c r="C6" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>128</v>
+      </c>
+      <c r="C7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A8">
+        <v>8</v>
+      </c>
+      <c r="B8" t="s">
+        <v>130</v>
+      </c>
+      <c r="C8" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="A9">
+        <v>9</v>
+      </c>
+      <c r="B9" t="s">
+        <v>132</v>
+      </c>
+      <c r="C9" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="28">
+        <v>10</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G11" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G12" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G13" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="G15" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new example, drawing a circle in realtime, and new functions, the general porpuse group of functions, used to calculate direct kinematics, and inverse kinematics of the KUKA iiwa 7 r 800 robot
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15220" windowHeight="6230" tabRatio="944" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="144">
   <si>
     <t>method</t>
   </si>
@@ -435,13 +435,34 @@
   </si>
   <si>
     <t>long test of the various funcitonalities of the toolbox</t>
+  </si>
+  <si>
+    <t>kuka0_moveRealtimeCircle</t>
+  </si>
+  <si>
+    <t>moving the robot in a circle in real time. Realtime motion planning and inverse kinematics is calculated in Matlab. At the same time the calculated joint angles are streamed to the robot, the robot moves the end-effector in a circle.</t>
+  </si>
+  <si>
+    <t>General porpuse</t>
+  </si>
+  <si>
+    <t>Calculating the inverse kinematics, joint angles from EEF transform.</t>
+  </si>
+  <si>
+    <t>Calculating the direct kinematics, EEF transfom, Jacobean.</t>
+  </si>
+  <si>
+    <t>directKinematics</t>
+  </si>
+  <si>
+    <t>kukaDLSSolver</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,6 +480,14 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -682,7 +711,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -738,6 +767,9 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -756,11 +788,21 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -768,74 +810,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -852,10 +826,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="CDE3DE"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1140,21 +1114,21 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B2" s="21" t="s">
+    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="23"/>
+      <c r="C2" s="23"/>
+      <c r="D2" s="23"/>
+      <c r="E2" s="23"/>
+      <c r="F2" s="23"/>
+      <c r="G2" s="23"/>
+      <c r="H2" s="23"/>
+      <c r="I2" s="23"/>
+      <c r="J2" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1173,7 +1147,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1187,12 +1161,12 @@
       <selection activeCell="B2" sqref="B2:C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="44.453125" customWidth="1"/>
+    <col min="2" max="3" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1200,7 +1174,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1211,7 +1185,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1235,12 +1209,12 @@
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="44.453125" customWidth="1"/>
+    <col min="2" max="3" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1248,7 +1222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1259,7 +1233,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1270,7 +1244,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1281,7 +1255,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1305,12 +1279,12 @@
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="44.453125" customWidth="1"/>
+    <col min="2" max="3" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1318,7 +1292,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1329,7 +1303,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1340,7 +1314,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1351,7 +1325,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1375,7 +1349,7 @@
       <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1389,12 +1363,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="44.453125" customWidth="1"/>
+    <col min="2" max="3" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1402,7 +1376,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1413,7 +1387,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1424,7 +1398,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1435,7 +1409,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1446,7 +1420,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1457,7 +1431,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1468,7 +1442,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1479,7 +1453,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1490,7 +1464,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1501,7 +1475,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1512,7 +1486,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1523,7 +1497,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1547,12 +1521,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="44.453125" customWidth="1"/>
+    <col min="2" max="3" width="44.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1560,7 +1534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1571,7 +1545,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
@@ -1583,7 +1557,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <f t="shared" ref="A4:A18" si="0">A3+1</f>
         <v>3</v>
@@ -1595,7 +1569,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1604,7 +1578,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1613,7 +1587,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1622,7 +1596,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1634,7 +1608,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1646,7 +1620,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1658,7 +1632,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1670,7 +1644,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1682,7 +1656,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1694,7 +1668,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1706,7 +1680,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1718,7 +1692,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -1730,7 +1704,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -1742,7 +1716,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -1762,35 +1736,35 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D55"/>
+  <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="C40" sqref="C38:C40"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C59" sqref="C59"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.81640625" customWidth="1"/>
-    <col min="2" max="2" width="17.90625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.36328125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="59.90625" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.77734375" customWidth="1"/>
+    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="59.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="C1" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B3" s="24" t="s">
+    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="26"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C3" s="26"/>
+      <c r="D3" s="27"/>
+    </row>
+    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B5" s="4" t="s">
         <v>68</v>
       </c>
@@ -1801,7 +1775,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1815,7 +1789,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>A6+1</f>
         <v>2</v>
@@ -1828,7 +1802,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
         <f t="shared" ref="A8:A55" si="0">A7+1</f>
         <v>3</v>
@@ -1843,7 +1817,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -1856,7 +1830,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -1869,7 +1843,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
@@ -1884,7 +1858,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
@@ -1897,7 +1871,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>8</v>
@@ -1910,7 +1884,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -1923,7 +1897,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>10</v>
@@ -1936,7 +1910,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>11</v>
@@ -1949,7 +1923,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="16" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>12</v>
@@ -1962,7 +1936,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="18" spans="1:4" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>13</v>
@@ -1975,7 +1949,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="19" spans="1:4" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>14</v>
@@ -1988,7 +1962,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="20" spans="1:4" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>15</v>
@@ -2001,7 +1975,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="16" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>16</v>
@@ -2014,7 +1988,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>17</v>
@@ -2029,7 +2003,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>18</v>
@@ -2042,7 +2016,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>19</v>
@@ -2055,7 +2029,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>20</v>
@@ -2068,7 +2042,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>21</v>
@@ -2081,7 +2055,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>22</v>
@@ -2094,7 +2068,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>23</v>
@@ -2107,7 +2081,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>24</v>
@@ -2120,7 +2094,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>25</v>
@@ -2133,7 +2107,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>26</v>
@@ -2146,7 +2120,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>27</v>
@@ -2159,7 +2133,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>28</v>
@@ -2172,7 +2146,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>29</v>
@@ -2185,7 +2159,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>30</v>
@@ -2200,7 +2174,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>31</v>
@@ -2213,7 +2187,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>32</v>
@@ -2226,7 +2200,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A38">
         <f t="shared" si="0"/>
         <v>33</v>
@@ -2239,7 +2213,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A39">
         <f t="shared" si="0"/>
         <v>34</v>
@@ -2252,7 +2226,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A40">
         <f t="shared" si="0"/>
         <v>35</v>
@@ -2265,7 +2239,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A41">
         <f t="shared" si="0"/>
         <v>36</v>
@@ -2278,7 +2252,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="58" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A42">
         <f t="shared" si="0"/>
         <v>37</v>
@@ -2291,7 +2265,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>38</v>
@@ -2302,7 +2276,7 @@
       </c>
       <c r="D43" s="8"/>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>39</v>
@@ -2313,7 +2287,7 @@
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2326,7 +2300,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2337,7 +2311,7 @@
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2350,7 +2324,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>43</v>
@@ -2363,7 +2337,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49">
         <f t="shared" si="0"/>
         <v>44</v>
@@ -2376,7 +2350,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A50">
         <f t="shared" si="0"/>
         <v>45</v>
@@ -2389,7 +2363,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A51">
         <f t="shared" si="0"/>
         <v>46</v>
@@ -2402,7 +2376,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>47</v>
@@ -2411,7 +2385,7 @@
       <c r="C52" s="3"/>
       <c r="D52" s="8"/>
     </row>
-    <row r="53" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>48</v>
@@ -2426,7 +2400,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A54">
         <f t="shared" si="0"/>
         <v>49</v>
@@ -2439,7 +2413,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55">
         <f t="shared" si="0"/>
         <v>50</v>
@@ -2450,6 +2424,26 @@
       </c>
       <c r="D55" s="12" t="s">
         <v>81</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B56" s="33" t="s">
+        <v>139</v>
+      </c>
+      <c r="C56" s="30" t="s">
+        <v>142</v>
+      </c>
+      <c r="D56" s="28" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B57" s="28"/>
+      <c r="C57" s="30" t="s">
+        <v>143</v>
+      </c>
+      <c r="D57" s="28" t="s">
+        <v>140</v>
       </c>
     </row>
   </sheetData>
@@ -2465,29 +2459,29 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.453125" customWidth="1"/>
-    <col min="2" max="2" width="35.453125" customWidth="1"/>
-    <col min="3" max="3" width="53.36328125" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="2" width="35.44140625" customWidth="1"/>
+    <col min="3" max="3" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1">
         <v>1</v>
       </c>
       <c r="B1" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="27" t="s">
+      <c r="C1" s="21" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>2</v>
       </c>
@@ -2498,7 +2492,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3</v>
       </c>
@@ -2509,7 +2503,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>4</v>
       </c>
@@ -2520,7 +2514,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>5</v>
       </c>
@@ -2531,7 +2525,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>6</v>
       </c>
@@ -2542,7 +2536,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>7</v>
       </c>
@@ -2553,7 +2547,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>8</v>
       </c>
@@ -2564,7 +2558,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>9</v>
       </c>
@@ -2575,38 +2569,47 @@
         <v>133</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="29" x14ac:dyDescent="0.35">
-      <c r="A10" s="28">
+    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A10" s="31">
         <v>10</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="32" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="29" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="31">
+        <v>11</v>
+      </c>
+      <c r="B11" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>138</v>
+      </c>
       <c r="G11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G13" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G14" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="G15" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
New example, controlling the end-effector of the KUKA iiwa using a gamepad
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="146">
   <si>
     <t>method</t>
   </si>
@@ -456,6 +456,12 @@
   </si>
   <si>
     <t>kukaDLSSolver</t>
+  </si>
+  <si>
+    <t>kuka0_gampade_EEFPosControl</t>
+  </si>
+  <si>
+    <t>example of integrating external hardware (gamepad) for real time conotrol of the end-effectpr of the robot.</t>
   </si>
 </sst>
 </file>
@@ -770,24 +776,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -803,6 +791,24 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1118,17 +1124,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="23"/>
-      <c r="D2" s="23"/>
-      <c r="E2" s="23"/>
-      <c r="F2" s="23"/>
-      <c r="G2" s="23"/>
-      <c r="H2" s="23"/>
-      <c r="I2" s="23"/>
-      <c r="J2" s="24"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="30"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1738,8 +1744,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C59" sqref="C59"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="D61" sqref="D61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1757,11 +1763,11 @@
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="25" t="s">
+      <c r="B3" s="31" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="27"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="33"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -2427,22 +2433,22 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B56" s="33" t="s">
+      <c r="B56" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="C56" s="30" t="s">
+      <c r="C56" s="24" t="s">
         <v>142</v>
       </c>
-      <c r="D56" s="28" t="s">
+      <c r="D56" s="22" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B57" s="28"/>
-      <c r="C57" s="30" t="s">
+      <c r="B57" s="22"/>
+      <c r="C57" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="D57" s="28" t="s">
+      <c r="D57" s="22" t="s">
         <v>140</v>
       </c>
     </row>
@@ -2459,8 +2465,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2570,31 +2576,40 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="31">
+      <c r="A10" s="25">
         <v>10</v>
       </c>
-      <c r="B10" s="32" t="s">
+      <c r="B10" s="26" t="s">
         <v>134</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="23" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="31">
+      <c r="A11" s="25">
         <v>11</v>
       </c>
-      <c r="B11" s="31" t="s">
+      <c r="B11" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="23" t="s">
         <v>138</v>
       </c>
       <c r="G11" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <v>12</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>145</v>
+      </c>
       <c r="G12" t="s">
         <v>113</v>
       </c>

</xml_diff>

<commit_message>
functions to calculate the direct/inverse dynamics and kinematics are added
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="146">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="158">
   <si>
     <t>method</t>
   </si>
@@ -449,19 +449,55 @@
     <t>Calculating the inverse kinematics, joint angles from EEF transform.</t>
   </si>
   <si>
-    <t>Calculating the direct kinematics, EEF transfom, Jacobean.</t>
-  </si>
-  <si>
-    <t>directKinematics</t>
-  </si>
-  <si>
-    <t>kukaDLSSolver</t>
-  </si>
-  <si>
     <t>kuka0_gampade_EEFPosControl</t>
   </si>
   <si>
     <t>example of integrating external hardware (gamepad) for real time conotrol of the end-effectpr of the robot.</t>
+  </si>
+  <si>
+    <t>gen_MassMatrix</t>
+  </si>
+  <si>
+    <t>gen_InverseDynamics</t>
+  </si>
+  <si>
+    <t>gen_GravityVector</t>
+  </si>
+  <si>
+    <t>gen_DirectDynamics</t>
+  </si>
+  <si>
+    <t>gen_CoriolisMatrix</t>
+  </si>
+  <si>
+    <t>gen_CentrifugalMatrix</t>
+  </si>
+  <si>
+    <t>Calculates the mass matrix of the manipulator</t>
+  </si>
+  <si>
+    <t>calculates the invers dynamics</t>
+  </si>
+  <si>
+    <t>calculates the torques vector due to gravity</t>
+  </si>
+  <si>
+    <t>calculates the direct kinematics</t>
+  </si>
+  <si>
+    <t>calculates the coriolis matrix</t>
+  </si>
+  <si>
+    <t>calculates the centrifugal matrix</t>
+  </si>
+  <si>
+    <t>gen_InverseKinematics</t>
+  </si>
+  <si>
+    <t>gen_DirectKinematics</t>
+  </si>
+  <si>
+    <t>Calculating the direct kinematics, EEF transfom/Jacobean matrices.</t>
   </si>
 </sst>
 </file>
@@ -816,6 +852,74 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -832,10 +936,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="CDE3DE"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="000000"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1742,10 +1846,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D57"/>
+  <dimension ref="A1:D63"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D61" sqref="D61"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1810,7 +1914,7 @@
     </row>
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" ref="A8:A55" si="0">A7+1</f>
+        <f t="shared" ref="A8:A63" si="0">A7+1</f>
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -2433,23 +2537,103 @@
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
       <c r="B56" s="27" t="s">
         <v>139</v>
       </c>
       <c r="C56" s="24" t="s">
-        <v>142</v>
+        <v>156</v>
       </c>
       <c r="D56" s="22" t="s">
-        <v>141</v>
+        <v>157</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
       <c r="B57" s="22"/>
       <c r="C57" s="24" t="s">
-        <v>143</v>
+        <v>155</v>
       </c>
       <c r="D57" s="22" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="C58" s="22" t="s">
+        <v>143</v>
+      </c>
+      <c r="D58" s="22" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="C59" s="22" t="s">
+        <v>144</v>
+      </c>
+      <c r="D59" s="22" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="C60" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="D60" s="22" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="C61" s="22" t="s">
+        <v>146</v>
+      </c>
+      <c r="D61" s="22" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="C62" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D62" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="C63" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>154</v>
       </c>
     </row>
   </sheetData>
@@ -2465,7 +2649,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+    <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
@@ -2605,10 +2789,10 @@
         <v>12</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="G12" t="s">
         <v>113</v>

</xml_diff>

<commit_message>
Precise hand guiding is integrated into the toolbox
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="158">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="164">
   <si>
     <t>method</t>
   </si>
@@ -498,6 +498,24 @@
   </si>
   <si>
     <t>Calculating the direct kinematics, EEF transfom/Jacobean matrices.</t>
+  </si>
+  <si>
+    <t>startPreciseHandGuiding</t>
+  </si>
+  <si>
+    <t>This function is used to start the precise hand guiding, this is a new functionality, it is not the same as the KUKA hand guiding. This functionality (controller) was created so that the user is able to precisely hand guide the robot at end-effector level.</t>
+  </si>
+  <si>
+    <t>kuka0_handGuidingExample</t>
+  </si>
+  <si>
+    <t>kuka0_preciseHandGuidingExample</t>
+  </si>
+  <si>
+    <t>an example for using the precise handguiding functionality, this is not the same as KUKA handguiding, this is a dedecated functionality (controller) that was establised to achieve precise hand guiding at end-effector level</t>
+  </si>
+  <si>
+    <t>an example on hand guiding</t>
   </si>
 </sst>
 </file>
@@ -569,7 +587,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -749,11 +767,54 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -825,9 +886,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -845,6 +903,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -852,74 +922,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -936,10 +938,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="CDE3DE"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="000000"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -1228,17 +1230,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="28" t="s">
+      <c r="B2" s="27" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="29"/>
-      <c r="E2" s="29"/>
-      <c r="F2" s="29"/>
-      <c r="G2" s="29"/>
-      <c r="H2" s="29"/>
-      <c r="I2" s="29"/>
-      <c r="J2" s="30"/>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="29"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1846,10 +1848,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D63"/>
+  <dimension ref="A1:D64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="C61" sqref="C61"/>
+    <sheetView tabSelected="1" topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="A64" sqref="A64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1867,11 +1869,11 @@
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="32"/>
-      <c r="D3" s="33"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="32"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1914,7 +1916,7 @@
     </row>
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" ref="A8:A63" si="0">A7+1</f>
+        <f t="shared" ref="A8:A64" si="0">A7+1</f>
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -2536,19 +2538,17 @@
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56">
+    <row r="56" spans="1:4" s="24" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="24">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B56" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C56" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="D56" s="22" t="s">
-        <v>157</v>
+      <c r="B56" s="34"/>
+      <c r="C56" s="35" t="s">
+        <v>158</v>
+      </c>
+      <c r="D56" s="36" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -2556,12 +2556,14 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B57" s="22"/>
+      <c r="B57" s="33" t="s">
+        <v>139</v>
+      </c>
       <c r="C57" s="24" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="D57" s="22" t="s">
-        <v>140</v>
+        <v>157</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -2569,11 +2571,12 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="C58" s="22" t="s">
-        <v>143</v>
+      <c r="B58" s="22"/>
+      <c r="C58" s="24" t="s">
+        <v>155</v>
       </c>
       <c r="D58" s="22" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2582,10 +2585,10 @@
         <v>54</v>
       </c>
       <c r="C59" s="22" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2594,10 +2597,10 @@
         <v>55</v>
       </c>
       <c r="C60" s="22" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2606,10 +2609,10 @@
         <v>56</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2618,10 +2621,10 @@
         <v>57</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2630,9 +2633,21 @@
         <v>58</v>
       </c>
       <c r="C63" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D63" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="C64" s="22" t="s">
         <v>148</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D64" s="22" t="s">
         <v>154</v>
       </c>
     </row>
@@ -2649,8 +2664,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2798,13 +2813,31 @@
         <v>113</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G13" t="s">
+    <row r="13" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <v>13</v>
+      </c>
+      <c r="B13" s="24" t="s">
+        <v>160</v>
+      </c>
+      <c r="C13" s="24" t="s">
+        <v>163</v>
+      </c>
+      <c r="G13" s="24" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G14" t="s">
+    <row r="14" spans="1:7" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
+        <v>14</v>
+      </c>
+      <c r="B14" s="25" t="s">
+        <v>161</v>
+      </c>
+      <c r="C14" s="23" t="s">
+        <v>162</v>
+      </c>
+      <c r="G14" s="24" t="s">
         <v>115</v>
       </c>
     </row>

</xml_diff>

<commit_message>
the (functions, script example) of realtime control with impedance is added to the functions list
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="172">
   <si>
     <t>method</t>
   </si>
@@ -522,6 +522,24 @@
   </si>
   <si>
     <t>calculates the partial jacobean</t>
+  </si>
+  <si>
+    <t>realTime_startImpedanceJoints.m</t>
+  </si>
+  <si>
+    <t>realTime_stopImpedanceJoints.m</t>
+  </si>
+  <si>
+    <t>start the realtime control with impedance</t>
+  </si>
+  <si>
+    <t>stop the realtime control with impedance</t>
+  </si>
+  <si>
+    <t>kuka0_realTimeImpedence.m</t>
+  </si>
+  <si>
+    <t>realtime control with impedance</t>
   </si>
 </sst>
 </file>
@@ -1854,10 +1872,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D65"/>
+  <dimension ref="A1:D158"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A54" workbookViewId="0">
-      <selection activeCell="A63" sqref="A63:A65"/>
+    <sheetView topLeftCell="A53" workbookViewId="0">
+      <selection activeCell="C67" sqref="C67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1922,7 +1940,7 @@
     </row>
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" ref="A8:A65" si="0">A7+1</f>
+        <f t="shared" ref="A8:A71" si="0">A7+1</f>
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -1961,19 +1979,17 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B11" s="7" t="s">
-        <v>73</v>
-      </c>
+      <c r="B11" s="9"/>
       <c r="C11" s="3" t="s">
-        <v>7</v>
+        <v>166</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>9</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1983,23 +1999,25 @@
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="D12" s="8" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B13" s="9"/>
+      <c r="B13" s="7" t="s">
+        <v>73</v>
+      </c>
       <c r="C13" s="3" t="s">
-        <v>61</v>
+        <v>7</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>64</v>
+        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
@@ -2009,10 +2027,10 @@
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="3" t="s">
-        <v>85</v>
+        <v>8</v>
       </c>
       <c r="D14" s="8" t="s">
-        <v>87</v>
+        <v>10</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
@@ -2022,10 +2040,10 @@
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="3" t="s">
-        <v>86</v>
+        <v>61</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>88</v>
+        <v>64</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.3">
@@ -2035,49 +2053,49 @@
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B17" s="9"/>
+      <c r="C17" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B18" s="9"/>
+      <c r="C18" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="D16" s="8" t="s">
+      <c r="D18" s="8" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="17" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B17" s="13"/>
-      <c r="C17" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B18" s="13"/>
-      <c r="C18" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B19" s="13"/>
       <c r="C19" s="14" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="20" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -2087,10 +2105,10 @@
       </c>
       <c r="B20" s="13"/>
       <c r="C20" s="14" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="D20" s="15" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
@@ -2100,38 +2118,36 @@
       </c>
       <c r="B21" s="13"/>
       <c r="C21" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21" s="15" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B22" s="13"/>
+      <c r="C22" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="D22" s="15" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B23" s="13"/>
+      <c r="C23" s="14" t="s">
         <v>96</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D23" s="15" t="s">
         <v>100</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B22" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B23" s="9"/>
-      <c r="C23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2139,38 +2155,40 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B24" s="9"/>
+      <c r="B24" s="7" t="s">
+        <v>72</v>
+      </c>
       <c r="C24" s="3" t="s">
-        <v>90</v>
+        <v>17</v>
       </c>
       <c r="D24" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B25" s="9"/>
       <c r="C25" s="3" t="s">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="D25" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B26" s="9"/>
       <c r="C26" s="3" t="s">
-        <v>42</v>
+        <v>90</v>
       </c>
       <c r="D26" s="8" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
@@ -2180,10 +2198,10 @@
       </c>
       <c r="B27" s="9"/>
       <c r="C27" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D27" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
@@ -2193,10 +2211,10 @@
       </c>
       <c r="B28" s="9"/>
       <c r="C28" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D28" s="8" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.3">
@@ -2206,10 +2224,10 @@
       </c>
       <c r="B29" s="9"/>
       <c r="C29" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D29" s="8" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
@@ -2219,10 +2237,10 @@
       </c>
       <c r="B30" s="9"/>
       <c r="C30" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D30" s="8" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
@@ -2232,10 +2250,10 @@
       </c>
       <c r="B31" s="9"/>
       <c r="C31" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D31" s="8" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.3">
@@ -2245,10 +2263,10 @@
       </c>
       <c r="B32" s="9"/>
       <c r="C32" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.3">
@@ -2258,10 +2276,10 @@
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.3">
@@ -2271,77 +2289,77 @@
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B35" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="B35" s="9"/>
       <c r="C35" s="3" t="s">
-        <v>20</v>
+        <v>49</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B38" s="9"/>
+      <c r="C38" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D36" s="8" t="s">
+      <c r="D38" s="8" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A37">
-        <f t="shared" si="0"/>
-        <v>32</v>
-      </c>
-      <c r="B37" s="9"/>
-      <c r="C37" s="3" t="s">
+    <row r="39" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B39" s="9"/>
+      <c r="C39" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="D37" s="8" t="s">
+      <c r="D39" s="8" t="s">
         <v>23</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A38">
-        <f t="shared" si="0"/>
-        <v>33</v>
-      </c>
-      <c r="B38" s="17"/>
-      <c r="C38" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D38" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A39">
-        <f t="shared" si="0"/>
-        <v>34</v>
-      </c>
-      <c r="B39" s="17"/>
-      <c r="C39" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="19" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
@@ -2351,59 +2369,63 @@
       </c>
       <c r="B40" s="17"/>
       <c r="C40" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D40" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B41" s="17"/>
+      <c r="C41" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D41" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B42" s="17"/>
+      <c r="C42" s="18" t="s">
         <v>108</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D42" s="19" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A41">
-        <f t="shared" si="0"/>
-        <v>36</v>
-      </c>
-      <c r="B41" s="9"/>
-      <c r="C41" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D41" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A42">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A43">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D43" s="8"/>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+      <c r="D43" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A44">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D44" s="8"/>
+        <v>28</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45">
@@ -2412,11 +2434,9 @@
       </c>
       <c r="B45" s="9"/>
       <c r="C45" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>33</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D45" s="8"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46">
@@ -2425,35 +2445,33 @@
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="3" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="D46" s="8"/>
     </row>
-    <row r="47" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A47">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A48">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
       <c r="B48" s="9"/>
       <c r="C48" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D48" s="8" t="s">
-        <v>40</v>
-      </c>
+        <v>34</v>
+      </c>
+      <c r="D48" s="8"/>
     </row>
     <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A49">
@@ -2462,7 +2480,7 @@
       </c>
       <c r="B49" s="9"/>
       <c r="C49" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D49" s="8" t="s">
         <v>40</v>
@@ -2475,7 +2493,7 @@
       </c>
       <c r="B50" s="9"/>
       <c r="C50" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D50" s="8" t="s">
         <v>40</v>
@@ -2488,34 +2506,36 @@
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D51" s="8" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A52">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B52" s="9"/>
-      <c r="C52" s="3"/>
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C52" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D52" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A53">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B53" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="B53" s="9"/>
       <c r="C53" s="3" t="s">
-        <v>76</v>
+        <v>39</v>
       </c>
       <c r="D53" s="8" t="s">
-        <v>79</v>
+        <v>40</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -2524,65 +2544,61 @@
         <v>49</v>
       </c>
       <c r="B54" s="9"/>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="3"/>
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B55" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D55" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B56" s="9"/>
+      <c r="C56" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D54" s="8" t="s">
+      <c r="D56" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A55">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B55" s="10"/>
-      <c r="C55" s="11" t="s">
+    <row r="57" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B57" s="10"/>
+      <c r="C57" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D55" s="12" t="s">
+      <c r="D57" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="56" spans="1:4" s="24" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="24">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B56" s="28"/>
-      <c r="C56" s="29" t="s">
+    <row r="58" spans="1:4" s="24" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B58" s="28"/>
+      <c r="C58" s="29" t="s">
         <v>158</v>
       </c>
-      <c r="D56" s="30" t="s">
+      <c r="D58" s="30" t="s">
         <v>159</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B57" s="27" t="s">
-        <v>139</v>
-      </c>
-      <c r="C57" s="24" t="s">
-        <v>156</v>
-      </c>
-      <c r="D57" s="22" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B58" s="22"/>
-      <c r="C58" s="24" t="s">
-        <v>155</v>
-      </c>
-      <c r="D58" s="22" t="s">
-        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2590,11 +2606,14 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="C59" s="22" t="s">
-        <v>143</v>
+      <c r="B59" s="27" t="s">
+        <v>139</v>
+      </c>
+      <c r="C59" s="24" t="s">
+        <v>156</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>149</v>
+        <v>157</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2602,11 +2621,12 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="C60" s="22" t="s">
-        <v>144</v>
+      <c r="B60" s="22"/>
+      <c r="C60" s="24" t="s">
+        <v>155</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2615,10 +2635,10 @@
         <v>56</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2627,10 +2647,10 @@
         <v>57</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2639,10 +2659,10 @@
         <v>58</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2651,10 +2671,10 @@
         <v>59</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2663,10 +2683,580 @@
         <v>60</v>
       </c>
       <c r="C65" s="22" t="s">
+        <v>147</v>
+      </c>
+      <c r="D65" s="22" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="C66" s="22" t="s">
+        <v>148</v>
+      </c>
+      <c r="D66" s="22" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="C67" s="22" t="s">
         <v>164</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="D67" s="22" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72">
+        <f t="shared" ref="A72:A135" si="1">A71+1</f>
+        <v>67</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A78">
+        <f t="shared" si="1"/>
+        <v>73</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A81">
+        <f t="shared" si="1"/>
+        <v>76</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A82">
+        <f t="shared" si="1"/>
+        <v>77</v>
+      </c>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A83">
+        <f t="shared" si="1"/>
+        <v>78</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A84">
+        <f t="shared" si="1"/>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A85">
+        <f t="shared" si="1"/>
+        <v>80</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A86">
+        <f t="shared" si="1"/>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A87">
+        <f t="shared" si="1"/>
+        <v>82</v>
+      </c>
+    </row>
+    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A88">
+        <f t="shared" si="1"/>
+        <v>83</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A89">
+        <f t="shared" si="1"/>
+        <v>84</v>
+      </c>
+    </row>
+    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A90">
+        <f t="shared" si="1"/>
+        <v>85</v>
+      </c>
+    </row>
+    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A91">
+        <f t="shared" si="1"/>
+        <v>86</v>
+      </c>
+    </row>
+    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A92">
+        <f t="shared" si="1"/>
+        <v>87</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A93">
+        <f t="shared" si="1"/>
+        <v>88</v>
+      </c>
+    </row>
+    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A94">
+        <f t="shared" si="1"/>
+        <v>89</v>
+      </c>
+    </row>
+    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A95">
+        <f t="shared" si="1"/>
+        <v>90</v>
+      </c>
+    </row>
+    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A96">
+        <f t="shared" si="1"/>
+        <v>91</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <f t="shared" si="1"/>
+        <v>92</v>
+      </c>
+    </row>
+    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <f t="shared" si="1"/>
+        <v>93</v>
+      </c>
+    </row>
+    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <f t="shared" si="1"/>
+        <v>94</v>
+      </c>
+    </row>
+    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <f t="shared" si="1"/>
+        <v>95</v>
+      </c>
+    </row>
+    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <f t="shared" si="1"/>
+        <v>96</v>
+      </c>
+    </row>
+    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A102">
+        <f t="shared" si="1"/>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A103">
+        <f t="shared" si="1"/>
+        <v>98</v>
+      </c>
+    </row>
+    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A104">
+        <f t="shared" si="1"/>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A105">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A106">
+        <f t="shared" si="1"/>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A107">
+        <f t="shared" si="1"/>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A108">
+        <f t="shared" si="1"/>
+        <v>103</v>
+      </c>
+    </row>
+    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A109">
+        <f t="shared" si="1"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A110">
+        <f t="shared" si="1"/>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A111">
+        <f t="shared" si="1"/>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A112">
+        <f t="shared" si="1"/>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A113">
+        <f t="shared" si="1"/>
+        <v>108</v>
+      </c>
+    </row>
+    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A114">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+    </row>
+    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A115">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+    </row>
+    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A116">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+    </row>
+    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A117">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+    </row>
+    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+    </row>
+    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A119">
+        <f t="shared" si="1"/>
+        <v>114</v>
+      </c>
+    </row>
+    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A120">
+        <f t="shared" si="1"/>
+        <v>115</v>
+      </c>
+    </row>
+    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A121">
+        <f t="shared" si="1"/>
+        <v>116</v>
+      </c>
+    </row>
+    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A122">
+        <f t="shared" si="1"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A123">
+        <f t="shared" si="1"/>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A124">
+        <f t="shared" si="1"/>
+        <v>119</v>
+      </c>
+    </row>
+    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A125">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
+    </row>
+    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A126">
+        <f t="shared" si="1"/>
+        <v>121</v>
+      </c>
+    </row>
+    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A127">
+        <f t="shared" si="1"/>
+        <v>122</v>
+      </c>
+    </row>
+    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A128">
+        <f t="shared" si="1"/>
+        <v>123</v>
+      </c>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A129">
+        <f t="shared" si="1"/>
+        <v>124</v>
+      </c>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A130">
+        <f t="shared" si="1"/>
+        <v>125</v>
+      </c>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A131">
+        <f t="shared" si="1"/>
+        <v>126</v>
+      </c>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A132">
+        <f t="shared" si="1"/>
+        <v>127</v>
+      </c>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A133">
+        <f t="shared" si="1"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A134">
+        <f t="shared" si="1"/>
+        <v>129</v>
+      </c>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A135">
+        <f t="shared" si="1"/>
+        <v>130</v>
+      </c>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A136">
+        <f t="shared" ref="A136:A158" si="2">A135+1</f>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A137">
+        <f t="shared" si="2"/>
+        <v>132</v>
+      </c>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A138">
+        <f t="shared" si="2"/>
+        <v>133</v>
+      </c>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A139">
+        <f t="shared" si="2"/>
+        <v>134</v>
+      </c>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A140">
+        <f t="shared" si="2"/>
+        <v>135</v>
+      </c>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A141">
+        <f t="shared" si="2"/>
+        <v>136</v>
+      </c>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A142">
+        <f t="shared" si="2"/>
+        <v>137</v>
+      </c>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A143">
+        <f t="shared" si="2"/>
+        <v>138</v>
+      </c>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A144">
+        <f t="shared" si="2"/>
+        <v>139</v>
+      </c>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A145">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A146">
+        <f t="shared" si="2"/>
+        <v>141</v>
+      </c>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A147">
+        <f t="shared" si="2"/>
+        <v>142</v>
+      </c>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A148">
+        <f t="shared" si="2"/>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A149">
+        <f t="shared" si="2"/>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A150">
+        <f t="shared" si="2"/>
+        <v>145</v>
+      </c>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A151">
+        <f t="shared" si="2"/>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A152">
+        <f t="shared" si="2"/>
+        <v>147</v>
+      </c>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A153">
+        <f t="shared" si="2"/>
+        <v>148</v>
+      </c>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A154">
+        <f t="shared" si="2"/>
+        <v>149</v>
+      </c>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A155">
+        <f t="shared" si="2"/>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A156">
+        <f t="shared" si="2"/>
+        <v>151</v>
+      </c>
+    </row>
+    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A157">
+        <f t="shared" si="2"/>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A158">
+        <f t="shared" si="2"/>
+        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -2682,8 +3272,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2860,6 +3450,15 @@
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
+        <v>15</v>
+      </c>
+      <c r="B15" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>171</v>
+      </c>
       <c r="G15" t="s">
         <v>116</v>
       </c>

</xml_diff>

<commit_message>
update the functions, add the ellipse example
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -362,21 +362,6 @@
     <t>returns the orientation of the end effector, it returns the rotation of the endeffector, relative to some defined frame. The returned rotation is expressed by a euler angles</t>
   </si>
   <si>
-    <t>with the KST for realtime control of the manipulator.</t>
-  </si>
-  <si>
-    <t>In this example the iiwa robot is controlled in realtime</t>
-  </si>
-  <si>
-    <t>using a gamepad controller, the example is in the folder</t>
-  </si>
-  <si>
-    <t>(realtimeControlOfJointSpaceUsingGamePad) of the github</t>
-  </si>
-  <si>
-    <t>repository.</t>
-  </si>
-  <si>
     <t xml:space="preserve">kuka0_circles: </t>
   </si>
   <si>
@@ -540,13 +525,28 @@
   </si>
   <si>
     <t>realtime control with impedance</t>
+  </si>
+  <si>
+    <t>kuka0_moveRealtimeEllipse.m</t>
+  </si>
+  <si>
+    <t>moving the robot on a ellipse in real time. Realtime motion planning and inverse kinematics is calculated in Matlab. At the same time the calculated joint angles are streamed to the robot, the robot moves the end-effector on the defined ellipse</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Example file name</t>
+  </si>
+  <si>
+    <t>About</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -572,6 +572,15 @@
     </font>
     <font>
       <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
@@ -838,7 +847,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -940,6 +949,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1986,10 +1996,10 @@
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="3" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
@@ -1999,10 +2009,10 @@
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="3" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
@@ -2595,10 +2605,10 @@
       </c>
       <c r="B58" s="28"/>
       <c r="C58" s="29" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="D58" s="30" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.3">
@@ -2607,13 +2617,13 @@
         <v>54</v>
       </c>
       <c r="B59" s="27" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="C59" s="24" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="D59" s="22" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.3">
@@ -2623,10 +2633,10 @@
       </c>
       <c r="B60" s="22"/>
       <c r="C60" s="24" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="D60" s="22" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.3">
@@ -2635,10 +2645,10 @@
         <v>56</v>
       </c>
       <c r="C61" s="22" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="D61" s="22" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -2647,10 +2657,10 @@
         <v>57</v>
       </c>
       <c r="C62" s="22" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="D62" s="22" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -2659,10 +2669,10 @@
         <v>58</v>
       </c>
       <c r="C63" s="22" t="s">
-        <v>145</v>
+        <v>140</v>
       </c>
       <c r="D63" s="22" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -2671,10 +2681,10 @@
         <v>59</v>
       </c>
       <c r="C64" s="22" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="D64" s="22" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -2683,10 +2693,10 @@
         <v>60</v>
       </c>
       <c r="C65" s="22" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D65" s="22" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -2695,10 +2705,10 @@
         <v>61</v>
       </c>
       <c r="C66" s="22" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="D66" s="22" t="s">
-        <v>154</v>
+        <v>149</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -2707,10 +2717,10 @@
         <v>62</v>
       </c>
       <c r="C67" s="22" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="D67" s="22" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -3270,10 +3280,10 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3283,184 +3293,191 @@
     <col min="3" max="3" width="53.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="37" t="s">
+        <v>170</v>
+      </c>
+      <c r="C1" s="37" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>112</v>
+      </c>
+      <c r="C2" s="21" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" t="s">
         <v>117</v>
       </c>
-      <c r="C1" s="21" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>118</v>
+      </c>
+      <c r="C5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>2</v>
-      </c>
-      <c r="B2" t="s">
-        <v>118</v>
-      </c>
-      <c r="C2" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>3</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="C6" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>121</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C7" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>123</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C8" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>5</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>125</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C10" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="25">
+        <v>10</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>129</v>
+      </c>
+      <c r="C11" s="23" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="25">
+        <v>11</v>
+      </c>
+      <c r="B12" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="C12" s="23" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A13" s="25">
+        <v>12</v>
+      </c>
+      <c r="B13" s="26" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>6</v>
-      </c>
-      <c r="B6" t="s">
-        <v>126</v>
-      </c>
-      <c r="C6" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
-        <v>128</v>
-      </c>
-      <c r="C7" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>8</v>
-      </c>
-      <c r="B8" t="s">
-        <v>130</v>
-      </c>
-      <c r="C8" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>9</v>
-      </c>
-      <c r="B9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C9" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A10" s="25">
-        <v>10</v>
-      </c>
-      <c r="B10" s="26" t="s">
-        <v>134</v>
-      </c>
-      <c r="C10" s="23" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
-        <v>11</v>
-      </c>
-      <c r="B11" s="25" t="s">
+      <c r="C13" s="23" t="s">
         <v>137</v>
       </c>
-      <c r="C11" s="23" t="s">
-        <v>138</v>
-      </c>
-      <c r="G11" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
-        <v>12</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>141</v>
-      </c>
-      <c r="C12" s="23" t="s">
-        <v>142</v>
-      </c>
-      <c r="G12" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
+    </row>
+    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="25">
         <v>13</v>
       </c>
-      <c r="B13" s="24" t="s">
-        <v>160</v>
-      </c>
-      <c r="C13" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
+      <c r="B14" s="24" t="s">
+        <v>155</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A15" s="25">
         <v>14</v>
       </c>
-      <c r="B14" s="25" t="s">
-        <v>161</v>
-      </c>
-      <c r="C14" s="23" t="s">
-        <v>162</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+      <c r="B15" s="25" t="s">
+        <v>156</v>
+      </c>
+      <c r="C15" s="23" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A16" s="25">
         <v>15</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>170</v>
-      </c>
-      <c r="C15" s="25" t="s">
-        <v>171</v>
-      </c>
-      <c r="G15" t="s">
-        <v>116</v>
+      <c r="B16" s="25" t="s">
+        <v>165</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A17" s="25">
+        <v>16</v>
+      </c>
+      <c r="B17" s="25" t="s">
+        <v>167</v>
+      </c>
+      <c r="C17" s="26" t="s">
+        <v>168</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add ellipse function list
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="188">
   <si>
     <t>method</t>
   </si>
@@ -540,6 +540,54 @@
   </si>
   <si>
     <t>About</t>
+  </si>
+  <si>
+    <t>movePTPEllipse</t>
+  </si>
+  <si>
+    <t>movePTPEllipseXY</t>
+  </si>
+  <si>
+    <t>movePTPEllipseXZ</t>
+  </si>
+  <si>
+    <t>movePTPEllipseYZ</t>
+  </si>
+  <si>
+    <t>movePTPEllipseImpedance</t>
+  </si>
+  <si>
+    <t>movePTPEllipseXYImpedance</t>
+  </si>
+  <si>
+    <t>movePTPEllipseXZImpedance</t>
+  </si>
+  <si>
+    <t>movePTPEllipseYZImpedance</t>
+  </si>
+  <si>
+    <t>Move the robot on an ellipse in 3D space</t>
+  </si>
+  <si>
+    <t>Move the robot on an ellipse in plane parallel to XY</t>
+  </si>
+  <si>
+    <t>Move the robot on an ellipse in plane parallel to XZ</t>
+  </si>
+  <si>
+    <t>Move the robot on an ellipse in plane parallel to YZ</t>
+  </si>
+  <si>
+    <t>Move the robot on an ellipse in 3D space, impedance control is enabled</t>
+  </si>
+  <si>
+    <t>Move the robot on an ellipse in plane parallel to XY, impedance control is enabled</t>
+  </si>
+  <si>
+    <t>Move the robot on an ellipse in plane parallel to XZ, impedance control is enabled</t>
+  </si>
+  <si>
+    <t>Move the robot on an ellipse in plane parallel to YZ, impedance control is enabled</t>
   </si>
 </sst>
 </file>
@@ -847,7 +895,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -931,6 +979,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -949,7 +1008,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1264,17 +1322,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="32"/>
-      <c r="D2" s="32"/>
-      <c r="E2" s="32"/>
-      <c r="F2" s="32"/>
-      <c r="G2" s="32"/>
-      <c r="H2" s="32"/>
-      <c r="I2" s="32"/>
-      <c r="J2" s="33"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
+      <c r="F2" s="37"/>
+      <c r="G2" s="37"/>
+      <c r="H2" s="37"/>
+      <c r="I2" s="37"/>
+      <c r="J2" s="38"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1882,10 +1940,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D158"/>
+  <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="C67" sqref="C67"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="D28" sqref="D28:D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1893,7 +1951,7 @@
     <col min="1" max="1" width="4.77734375" customWidth="1"/>
     <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
     <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="59.88671875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="68.88671875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
@@ -1903,11 +1961,11 @@
     </row>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="34" t="s">
+      <c r="B3" s="39" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="35"/>
-      <c r="D3" s="36"/>
+      <c r="C3" s="40"/>
+      <c r="D3" s="41"/>
     </row>
     <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
@@ -1950,7 +2008,7 @@
     </row>
     <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" ref="A8:A71" si="0">A7+1</f>
+        <f t="shared" ref="A8:A79" si="0">A7+1</f>
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
@@ -2160,1113 +2218,899 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A24">
+    <row r="24" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="32"/>
+      <c r="C24" s="33" t="s">
+        <v>172</v>
+      </c>
+      <c r="D24" s="34" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="20">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B25" s="32"/>
+      <c r="C25" s="33" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25" s="34" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="20">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B26" s="32"/>
+      <c r="C26" s="33" t="s">
+        <v>174</v>
+      </c>
+      <c r="D26" s="34" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="20">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B27" s="32"/>
+      <c r="C27" s="33" t="s">
+        <v>175</v>
+      </c>
+      <c r="D27" s="34" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B28" s="32"/>
+      <c r="C28" s="33" t="s">
+        <v>176</v>
+      </c>
+      <c r="D28" s="34" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="32"/>
+      <c r="C29" s="33" t="s">
+        <v>177</v>
+      </c>
+      <c r="D29" s="34" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B30" s="32"/>
+      <c r="C30" s="33" t="s">
+        <v>178</v>
+      </c>
+      <c r="D30" s="34" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B31" s="32"/>
+      <c r="C31" s="33" t="s">
+        <v>179</v>
+      </c>
+      <c r="D31" s="34" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A32" s="20">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B32" s="7" t="s">
         <v>72</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="8" t="s">
+      <c r="D32" s="8" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A25">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B25" s="9"/>
-      <c r="C25" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D25" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A26">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B26" s="9"/>
-      <c r="C26" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A27">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B27" s="9"/>
-      <c r="C27" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A28">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A29">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B29" s="9"/>
-      <c r="C29" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A30">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B30" s="9"/>
-      <c r="C30" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="D30" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A31">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B31" s="9"/>
-      <c r="C31" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="D31" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A32">
-        <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="B32" s="9"/>
-      <c r="C32" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A33">
+    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A33" s="20">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
       <c r="B33" s="9"/>
       <c r="C33" s="3" t="s">
-        <v>47</v>
+        <v>18</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A34">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A34" s="20">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="3" t="s">
-        <v>48</v>
+        <v>90</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>57</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35">
+      <c r="A35" s="20">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="3" t="s">
-        <v>49</v>
+        <v>41</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36">
+      <c r="A36" s="20">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="3" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A37">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A37" s="20">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B37" s="7" t="s">
-        <v>74</v>
-      </c>
+      <c r="B37" s="9"/>
       <c r="C37" s="3" t="s">
-        <v>20</v>
+        <v>43</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A38" s="20">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="3" t="s">
-        <v>21</v>
+        <v>44</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A39">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A39" s="20">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="3" t="s">
-        <v>83</v>
+        <v>45</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A40">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A40" s="20">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B40" s="17"/>
-      <c r="C40" s="18" t="s">
-        <v>107</v>
-      </c>
-      <c r="D40" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A41">
+      <c r="B40" s="9"/>
+      <c r="C40" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D40" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A41" s="20">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B41" s="17"/>
-      <c r="C41" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A42">
+      <c r="B41" s="9"/>
+      <c r="C41" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A42" s="20">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B42" s="17"/>
-      <c r="C42" s="18" t="s">
-        <v>108</v>
-      </c>
-      <c r="D42" s="19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A43">
+      <c r="B42" s="9"/>
+      <c r="C42" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D42" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A43" s="20">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="3" t="s">
-        <v>84</v>
+        <v>49</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A44">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A44" s="20">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="3" t="s">
-        <v>28</v>
+        <v>50</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A45" s="20">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B45" s="9"/>
+      <c r="B45" s="7" t="s">
+        <v>74</v>
+      </c>
       <c r="C45" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D45" s="8"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46">
+        <v>20</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A46" s="20">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D46" s="8"/>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A47">
+        <v>21</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A47" s="20">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="3" t="s">
-        <v>32</v>
+        <v>83</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A48">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A48" s="20">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B48" s="9"/>
-      <c r="C48" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D48" s="8"/>
-    </row>
-    <row r="49" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A49">
+      <c r="B48" s="17"/>
+      <c r="C48" s="18" t="s">
+        <v>107</v>
+      </c>
+      <c r="D48" s="19" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A49" s="20">
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B49" s="9"/>
-      <c r="C49" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D49" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A50">
+      <c r="B49" s="17"/>
+      <c r="C49" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="D49" s="19" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A50" s="20">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B50" s="9"/>
-      <c r="C50" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D50" s="8" t="s">
-        <v>40</v>
+      <c r="B50" s="17"/>
+      <c r="C50" s="18" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" s="19" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51">
+      <c r="A51" s="20">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="3" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A52">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A52" s="20">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="3" t="s">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D52" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A53">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A53" s="20">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="D53" s="8" t="s">
-        <v>40</v>
-      </c>
+        <v>30</v>
+      </c>
+      <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54">
+      <c r="A54" s="20">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B54" s="9"/>
-      <c r="C54" s="3"/>
+      <c r="C54" s="3" t="s">
+        <v>31</v>
+      </c>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A55">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A55" s="20">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B55" s="7" t="s">
-        <v>75</v>
-      </c>
+      <c r="B55" s="9"/>
       <c r="C55" s="3" t="s">
-        <v>76</v>
+        <v>32</v>
       </c>
       <c r="D55" s="8" t="s">
-        <v>79</v>
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56">
+      <c r="A56" s="20">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A57" s="20">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B57" s="9"/>
+      <c r="C57" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D57" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A58" s="20">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B58" s="9"/>
+      <c r="C58" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D58" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A59" s="20">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B59" s="9"/>
+      <c r="C59" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D59" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A60" s="20">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B60" s="9"/>
+      <c r="C60" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D60" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A61" s="20">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B61" s="9"/>
+      <c r="C61" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D61" s="8" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A62" s="20">
+        <f t="shared" si="0"/>
+        <v>57</v>
+      </c>
+      <c r="B62" s="9"/>
+      <c r="C62" s="3"/>
+      <c r="D62" s="8"/>
+    </row>
+    <row r="63" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A63" s="20">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B63" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="D63" s="8" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A64" s="20">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B64" s="9"/>
+      <c r="C64" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="D56" s="8" t="s">
+      <c r="D64" s="8" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A57">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B57" s="10"/>
-      <c r="C57" s="11" t="s">
+    <row r="65" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A65" s="20">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B65" s="10"/>
+      <c r="C65" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="D57" s="12" t="s">
+      <c r="D65" s="12" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="58" spans="1:4" s="24" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A58">
-        <f t="shared" si="0"/>
-        <v>53</v>
-      </c>
-      <c r="B58" s="28"/>
-      <c r="C58" s="29" t="s">
+    <row r="66" spans="1:4" s="24" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A66" s="20">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B66" s="28"/>
+      <c r="C66" s="29" t="s">
         <v>153</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D66" s="30" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A59">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B59" s="27" t="s">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A67" s="20">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B67" s="27" t="s">
         <v>134</v>
       </c>
-      <c r="C59" s="24" t="s">
+      <c r="C67" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="D59" s="22" t="s">
+      <c r="D67" s="22" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A60">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B60" s="22"/>
-      <c r="C60" s="24" t="s">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A68" s="20">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B68" s="22"/>
+      <c r="C68" s="24" t="s">
         <v>150</v>
       </c>
-      <c r="D60" s="22" t="s">
+      <c r="D68" s="22" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A61">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="C61" s="22" t="s">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A69" s="20">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C69" s="22" t="s">
         <v>138</v>
       </c>
-      <c r="D61" s="22" t="s">
+      <c r="D69" s="22" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="C62" s="22" t="s">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A70" s="20">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C70" s="22" t="s">
         <v>139</v>
       </c>
-      <c r="D62" s="22" t="s">
+      <c r="D70" s="22" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A63">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="C63" s="22" t="s">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A71" s="20">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="C71" s="22" t="s">
         <v>140</v>
       </c>
-      <c r="D63" s="22" t="s">
+      <c r="D71" s="22" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="C64" s="22" t="s">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A72" s="20">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="C72" s="22" t="s">
         <v>141</v>
       </c>
-      <c r="D64" s="22" t="s">
+      <c r="D72" s="22" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A65">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="C65" s="22" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A73" s="20">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="C73" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="D65" s="22" t="s">
+      <c r="D73" s="22" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A66">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="C66" s="22" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A74" s="20">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C74" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="22" t="s">
+      <c r="D74" s="22" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="C67" s="22" t="s">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A75" s="20">
+        <f t="shared" si="0"/>
+        <v>70</v>
+      </c>
+      <c r="C75" s="22" t="s">
         <v>159</v>
       </c>
-      <c r="D67" s="22" t="s">
+      <c r="D75" s="22" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72">
-        <f t="shared" ref="A72:A135" si="1">A71+1</f>
-        <v>67</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73">
-        <f t="shared" si="1"/>
-        <v>68</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74">
-        <f t="shared" si="1"/>
-        <v>69</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75">
-        <f t="shared" si="1"/>
-        <v>70</v>
-      </c>
-    </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76">
-        <f t="shared" si="1"/>
+      <c r="A76" s="20">
+        <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77">
-        <f t="shared" si="1"/>
+      <c r="A77" s="20">
+        <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78">
-        <f t="shared" si="1"/>
+      <c r="A78" s="20">
+        <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79">
-        <f t="shared" si="1"/>
+      <c r="A79" s="20">
+        <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80">
-        <f t="shared" si="1"/>
+      <c r="A80" s="20">
+        <f t="shared" ref="A80:A113" si="1">A79+1</f>
         <v>75</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81">
+      <c r="A81" s="20">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82">
+      <c r="A82" s="20">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83">
+      <c r="A83" s="20">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
     <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84">
+      <c r="A84" s="20">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
     </row>
     <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85">
+      <c r="A85" s="20">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
     <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86">
+      <c r="A86" s="20">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
     <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87">
+      <c r="A87" s="20">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
     <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88">
+      <c r="A88" s="20">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89">
+      <c r="A89" s="20">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90">
+      <c r="A90" s="20">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
     <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91">
+      <c r="A91" s="20">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
     <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92">
+      <c r="A92" s="20">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
     <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93">
+      <c r="A93" s="20">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
     </row>
     <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94">
+      <c r="A94" s="20">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
     </row>
     <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95">
+      <c r="A95" s="20">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
     <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96">
+      <c r="A96" s="20">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
     </row>
     <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97">
+      <c r="A97" s="20">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
     <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98">
+      <c r="A98" s="20">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
     <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99">
+      <c r="A99" s="20">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
     </row>
     <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100">
+      <c r="A100" s="20">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
     </row>
     <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101">
+      <c r="A101" s="20">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
     </row>
     <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102">
+      <c r="A102" s="20">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
     </row>
     <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103">
+      <c r="A103" s="20">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
     </row>
     <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104">
+      <c r="A104" s="20">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
     </row>
     <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105">
+      <c r="A105" s="20">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106">
+      <c r="A106" s="20">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107">
+      <c r="A107" s="20">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
     </row>
     <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108">
+      <c r="A108" s="20">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
     </row>
     <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109">
+      <c r="A109" s="20">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
     <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110">
+      <c r="A110" s="20">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111">
+      <c r="A111" s="20">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
     </row>
     <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112">
+      <c r="A112" s="20">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113">
+      <c r="A113" s="20">
         <f t="shared" si="1"/>
         <v>108</v>
-      </c>
-    </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A114">
-        <f t="shared" si="1"/>
-        <v>109</v>
-      </c>
-    </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A115">
-        <f t="shared" si="1"/>
-        <v>110</v>
-      </c>
-    </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A116">
-        <f t="shared" si="1"/>
-        <v>111</v>
-      </c>
-    </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A117">
-        <f t="shared" si="1"/>
-        <v>112</v>
-      </c>
-    </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A118">
-        <f t="shared" si="1"/>
-        <v>113</v>
-      </c>
-    </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A119">
-        <f t="shared" si="1"/>
-        <v>114</v>
-      </c>
-    </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A120">
-        <f t="shared" si="1"/>
-        <v>115</v>
-      </c>
-    </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A121">
-        <f t="shared" si="1"/>
-        <v>116</v>
-      </c>
-    </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A122">
-        <f t="shared" si="1"/>
-        <v>117</v>
-      </c>
-    </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A123">
-        <f t="shared" si="1"/>
-        <v>118</v>
-      </c>
-    </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A124">
-        <f t="shared" si="1"/>
-        <v>119</v>
-      </c>
-    </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A125">
-        <f t="shared" si="1"/>
-        <v>120</v>
-      </c>
-    </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A126">
-        <f t="shared" si="1"/>
-        <v>121</v>
-      </c>
-    </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A127">
-        <f t="shared" si="1"/>
-        <v>122</v>
-      </c>
-    </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A128">
-        <f t="shared" si="1"/>
-        <v>123</v>
-      </c>
-    </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A129">
-        <f t="shared" si="1"/>
-        <v>124</v>
-      </c>
-    </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A130">
-        <f t="shared" si="1"/>
-        <v>125</v>
-      </c>
-    </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A131">
-        <f t="shared" si="1"/>
-        <v>126</v>
-      </c>
-    </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A132">
-        <f t="shared" si="1"/>
-        <v>127</v>
-      </c>
-    </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A133">
-        <f t="shared" si="1"/>
-        <v>128</v>
-      </c>
-    </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A134">
-        <f t="shared" si="1"/>
-        <v>129</v>
-      </c>
-    </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A135">
-        <f t="shared" si="1"/>
-        <v>130</v>
-      </c>
-    </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A136">
-        <f t="shared" ref="A136:A158" si="2">A135+1</f>
-        <v>131</v>
-      </c>
-    </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A137">
-        <f t="shared" si="2"/>
-        <v>132</v>
-      </c>
-    </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A138">
-        <f t="shared" si="2"/>
-        <v>133</v>
-      </c>
-    </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A139">
-        <f t="shared" si="2"/>
-        <v>134</v>
-      </c>
-    </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A140">
-        <f t="shared" si="2"/>
-        <v>135</v>
-      </c>
-    </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A141">
-        <f t="shared" si="2"/>
-        <v>136</v>
-      </c>
-    </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A142">
-        <f t="shared" si="2"/>
-        <v>137</v>
-      </c>
-    </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A143">
-        <f t="shared" si="2"/>
-        <v>138</v>
-      </c>
-    </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A144">
-        <f t="shared" si="2"/>
-        <v>139</v>
-      </c>
-    </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A145">
-        <f t="shared" si="2"/>
-        <v>140</v>
-      </c>
-    </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A146">
-        <f t="shared" si="2"/>
-        <v>141</v>
-      </c>
-    </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A147">
-        <f t="shared" si="2"/>
-        <v>142</v>
-      </c>
-    </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A148">
-        <f t="shared" si="2"/>
-        <v>143</v>
-      </c>
-    </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A149">
-        <f t="shared" si="2"/>
-        <v>144</v>
-      </c>
-    </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A150">
-        <f t="shared" si="2"/>
-        <v>145</v>
-      </c>
-    </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A151">
-        <f t="shared" si="2"/>
-        <v>146</v>
-      </c>
-    </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A152">
-        <f t="shared" si="2"/>
-        <v>147</v>
-      </c>
-    </row>
-    <row r="153" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A153">
-        <f t="shared" si="2"/>
-        <v>148</v>
-      </c>
-    </row>
-    <row r="154" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A154">
-        <f t="shared" si="2"/>
-        <v>149</v>
-      </c>
-    </row>
-    <row r="155" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A155">
-        <f t="shared" si="2"/>
-        <v>150</v>
-      </c>
-    </row>
-    <row r="156" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A156">
-        <f t="shared" si="2"/>
-        <v>151</v>
-      </c>
-    </row>
-    <row r="157" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A157">
-        <f t="shared" si="2"/>
-        <v>152</v>
-      </c>
-    </row>
-    <row r="158" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A158">
-        <f t="shared" si="2"/>
-        <v>153</v>
       </c>
     </row>
   </sheetData>
@@ -3282,8 +3126,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3294,13 +3138,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="37" t="s">
+      <c r="A1" s="31" t="s">
         <v>169</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="31" t="s">
         <v>170</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="31" t="s">
         <v>171</v>
       </c>
     </row>

</xml_diff>

<commit_message>
new functions added, KST 1.2
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" firstSheet="4" activeTab="7"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="268" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="196">
   <si>
     <t>method</t>
   </si>
@@ -588,6 +588,30 @@
   </si>
   <si>
     <t>Move the robot on an ellipse in plane parallel to YZ, impedance control is enabled</t>
+  </si>
+  <si>
+    <t>sendJointsPositionsExTorque</t>
+  </si>
+  <si>
+    <t>modify the joint positions of the robot, returns back external torques, applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>sendJointsPositionsMTorque</t>
+  </si>
+  <si>
+    <t>modify the joint positions of the robot,, returns back measured torques applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>sendJointsPositionsGetActualJpos</t>
+  </si>
+  <si>
+    <t>modify the joint positions of the robot, returns back joint position measurments from encoders, applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>sendJointsPositionsGetActualEEFpos</t>
+  </si>
+  <si>
+    <t>modify the joint positions of the robot, returns back EEF position measurments from robot applicable only in real-time motion</t>
   </si>
 </sst>
 </file>
@@ -895,7 +919,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1007,6 +1031,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1407,10 +1437,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1468,6 +1498,50 @@
       </c>
       <c r="C5" t="s">
         <v>101</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="42" t="s">
+        <v>188</v>
+      </c>
+      <c r="C6" s="43" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="42" t="s">
+        <v>190</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="42" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="43" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="42" t="s">
+        <v>194</v>
+      </c>
+      <c r="C9" s="43" t="s">
+        <v>195</v>
       </c>
     </row>
   </sheetData>
@@ -1942,7 +2016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView topLeftCell="A52" workbookViewId="0">
       <selection activeCell="D28" sqref="D28:D31"/>
     </sheetView>
   </sheetViews>
@@ -2493,7 +2567,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A45" s="20">
         <f t="shared" si="0"/>
         <v>40</v>
@@ -2508,7 +2582,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="46" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A46" s="20">
         <f t="shared" si="0"/>
         <v>41</v>
@@ -2521,7 +2595,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A47" s="20">
         <f t="shared" si="0"/>
         <v>42</v>
@@ -2586,7 +2660,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A52" s="20">
         <f t="shared" si="0"/>
         <v>47</v>

</xml_diff>

<commit_message>
read me, functions list updated
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15216" windowHeight="6228" tabRatio="944" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11385" windowHeight="10125" tabRatio="944" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -18,12 +18,12 @@
     <sheet name="exmple files" sheetId="7" r:id="rId9"/>
     <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="196">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="250">
   <si>
     <t>method</t>
   </si>
@@ -80,9 +80,6 @@
   </si>
   <si>
     <t>sendJointsPositions</t>
-  </si>
-  <si>
-    <t>update the parameters of the memory, that holds the cartizian positions of the end-effector.</t>
   </si>
   <si>
     <t>getEEF_Force</t>
@@ -329,12 +326,6 @@
     <t>moves the robot in an arc in the YZ plane, the arc is specified by the Y and Z position of its center and the angle subtended by the arc from the center.</t>
   </si>
   <si>
-    <t>Update the joints positions</t>
-  </si>
-  <si>
-    <t>update the parameters of the memory, that holds the joint positions.</t>
-  </si>
-  <si>
     <t xml:space="preserve">returns the external torques of the joints, for more information refer to matlab file (getJointsExternalTorques.m) </t>
   </si>
   <si>
@@ -593,32 +584,203 @@
     <t>sendJointsPositionsExTorque</t>
   </si>
   <si>
-    <t>modify the joint positions of the robot, returns back external torques, applicable only in real-time motion</t>
-  </si>
-  <si>
     <t>sendJointsPositionsMTorque</t>
   </si>
   <si>
-    <t>modify the joint positions of the robot,, returns back measured torques applicable only in real-time motion</t>
-  </si>
-  <si>
     <t>sendJointsPositionsGetActualJpos</t>
   </si>
   <si>
-    <t>modify the joint positions of the robot, returns back joint position measurments from encoders, applicable only in real-time motion</t>
-  </si>
-  <si>
     <t>sendJointsPositionsGetActualEEFpos</t>
   </si>
   <si>
-    <t>modify the joint positions of the robot, returns back EEF position measurments from robot applicable only in real-time motion</t>
+    <t>send distintation position for the joints of the robot, returns back external torques, applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send distintation position for the joints of the robot, returns back measured torques applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send distintation position for the joints of the robot, returns back joint position measurments from encoders, applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send distintation position for the joints of the robot returns back EEF position measurments from robot applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>sendEEfPositionMTorque</t>
+  </si>
+  <si>
+    <t>sendEEfPositionGetActualJpos</t>
+  </si>
+  <si>
+    <t>sendEEfPositionGetActualEEFpos</t>
+  </si>
+  <si>
+    <t>sendEEfPositionExTorque</t>
+  </si>
+  <si>
+    <t>Send distination position for joints angles, and waits for the acknowledgment that the message has been processed</t>
+  </si>
+  <si>
+    <t>net_updateDelay</t>
+  </si>
+  <si>
+    <t>Establish a plot of comunication delay between PC and controller</t>
+  </si>
+  <si>
+    <t>nonBlocking_movePTPLineEEF</t>
+  </si>
+  <si>
+    <t>nonBlocking_movePTPHomeJointSpace</t>
+  </si>
+  <si>
+    <t>nonBlocking_movePTPCirc1OrintationInter</t>
+  </si>
+  <si>
+    <t>nonBlocking_movePTPArcYZ_AC</t>
+  </si>
+  <si>
+    <t>nonBlocking_movePTPArcXZ_AC</t>
+  </si>
+  <si>
+    <t>nonBlocking_movePTPArcXY_AC</t>
+  </si>
+  <si>
+    <t>nonBlocking_movePTPArc_AC</t>
+  </si>
+  <si>
+    <t>nonBlocking_isGoalReached</t>
+  </si>
+  <si>
+    <t>nonBlocking_movePTPTransportPositionJointSpace</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_Arc_AC</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_LineEEF</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_LineEefRelBase</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_JointSpace</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_Circ1OrintationInter</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_ArcYZ_AC</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_ArcXZ_AC</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_ArcXY_AC</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_HomeJointSpace</t>
+  </si>
+  <si>
+    <t>movePTP_ConditionalTorque_TransportPositionJointSpace</t>
+  </si>
+  <si>
+    <t>realTime_startDirectServoCartesian</t>
+  </si>
+  <si>
+    <t>realTime_stopDirectServoCartesian</t>
+  </si>
+  <si>
+    <t>sendEEfPosition</t>
+  </si>
+  <si>
+    <t>sendEEfPositionf</t>
+  </si>
+  <si>
+    <t>net_pinIIWA</t>
+  </si>
+  <si>
+    <t>Ping the controller</t>
+  </si>
+  <si>
+    <t>realTime_startVelControlJoints</t>
+  </si>
+  <si>
+    <t>realTime_stopVelControlJoints</t>
+  </si>
+  <si>
+    <t>sendJointsVelocities</t>
+  </si>
+  <si>
+    <t>sendJointsVelocitiesExTorques</t>
+  </si>
+  <si>
+    <t>sendJointsVelocitiesMTorques</t>
+  </si>
+  <si>
+    <t>sendJointsVelocitiesGetActualJpos</t>
+  </si>
+  <si>
+    <t>sendJointsVelocitiesGetActualEEfPos</t>
+  </si>
+  <si>
+    <t>send distintation position for the EEF of the robot, returns back external torques, applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send distintation position for the EEF of the robot, returns back measured torques applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send distintation position for the EEF of the robot, returns back joint position measurments from encoders, applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send distintation position for the EEF of the robot returns back EEF position measurments from robot applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>Send distnination position for joints angles to the robot,</t>
+  </si>
+  <si>
+    <t>start the soft real time control in joint velocity mod</t>
+  </si>
+  <si>
+    <t>stop the soft real time control in joint velocity mod</t>
+  </si>
+  <si>
+    <t>Send reference velocities for joints of the robot,</t>
+  </si>
+  <si>
+    <t>send reference velocities for the joints of the robot, returns back external torques, applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send reference velocities for the joints of the robot, returns back measured torques applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send reference velocities for the joints of the robot, returns back joint position measurments from encoders, applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>send reference velocities for the joints of the robot returns back EEF position measurments from robot applicable only in real-time motion</t>
+  </si>
+  <si>
+    <t>Tutorial_softRealTimeJointsVelControl</t>
+  </si>
+  <si>
+    <t>Tutorial_realTimeImpedencePlotTorqueFeedBack</t>
+  </si>
+  <si>
+    <t>Tutorial_ptpPickPlacePhysicalInteraction</t>
+  </si>
+  <si>
+    <t>Pick and place with phisical human interaction</t>
+  </si>
+  <si>
+    <t>Move joints in realtime using impedence, plot torque feedback</t>
+  </si>
+  <si>
+    <t>´Realtime control using joint space velocity control mode</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -659,6 +821,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -687,7 +857,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -919,7 +1089,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -955,16 +1125,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1004,16 +1164,30 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1032,10 +1206,7 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1348,21 +1519,21 @@
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:10" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="36" t="s">
+    <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="38" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="37"/>
-      <c r="I2" s="37"/>
-      <c r="J2" s="38"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="40"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1381,7 +1552,7 @@
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1389,18 +1560,18 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="3" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1408,26 +1579,50 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="32" t="s">
         <v>3</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="32" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="32" t="s">
         <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f>A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>198</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C5" s="32" t="s">
+        <v>224</v>
       </c>
     </row>
   </sheetData>
@@ -1437,18 +1632,19 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:A9"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="2" width="44.42578125" customWidth="1"/>
+    <col min="3" max="3" width="55.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1456,92 +1652,307 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A27" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="C7" s="3"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>220</v>
+      </c>
+      <c r="C8" s="3"/>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C5" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" s="42" t="s">
+      <c r="C9" s="3" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>221</v>
+      </c>
+      <c r="C11" s="3"/>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>222</v>
+      </c>
+      <c r="C12" s="3"/>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="28" t="s">
+        <v>185</v>
+      </c>
+      <c r="C13" s="29" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="28" t="s">
+        <v>186</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="28" t="s">
+        <v>187</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="28" t="s">
         <v>188</v>
       </c>
-      <c r="C6" s="43" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" s="42" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="43" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" s="42" t="s">
+      <c r="C16" s="29" t="s">
         <v>192</v>
       </c>
-      <c r="C8" s="43" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="36" t="s">
+        <v>196</v>
+      </c>
+      <c r="C17" s="37" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="36" t="s">
         <v>193</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" s="42" t="s">
+      <c r="C18" s="37" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="36" t="s">
         <v>194</v>
       </c>
-      <c r="C9" s="43" t="s">
+      <c r="C19" s="37" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="36" t="s">
         <v>195</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>225</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>226</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>227</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>228</v>
+      </c>
+      <c r="C24" s="28" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>229</v>
+      </c>
+      <c r="C25" s="28" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>230</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>231</v>
+      </c>
+      <c r="C27" s="28" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -1551,68 +1962,418 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B43" sqref="B43"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="2" width="59.28515625" customWidth="1"/>
+    <col min="3" max="3" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="32" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>1+A2</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="32" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A37" si="0">1+A3</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C4" s="32" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="32" t="s">
         <v>61</v>
       </c>
-      <c r="C4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="C5" t="s">
-        <v>63</v>
-      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="C6" s="32" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="32" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="32" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="C11" s="32" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="C12" s="32" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="C13" s="32" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="C14" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>173</v>
+      </c>
+      <c r="C15" s="32" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C16" s="32" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="32" t="s">
+        <v>175</v>
+      </c>
+      <c r="C17" s="32" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="32" t="s">
+        <v>176</v>
+      </c>
+      <c r="C18" s="32" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="34" t="s">
+        <v>200</v>
+      </c>
+      <c r="C19" s="34"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="34" t="s">
+        <v>202</v>
+      </c>
+      <c r="C20" s="34"/>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B21" s="34" t="s">
+        <v>203</v>
+      </c>
+      <c r="C21" s="34"/>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B22" s="34" t="s">
+        <v>204</v>
+      </c>
+      <c r="C22" s="34"/>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B23" s="34" t="s">
+        <v>205</v>
+      </c>
+      <c r="C23" s="34"/>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B24" s="34" t="s">
+        <v>206</v>
+      </c>
+      <c r="C24" s="34"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B25" s="34" t="s">
+        <v>207</v>
+      </c>
+      <c r="C25" s="34"/>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B26" s="34" t="s">
+        <v>208</v>
+      </c>
+      <c r="C26" s="34"/>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B27" s="34" t="s">
+        <v>201</v>
+      </c>
+      <c r="C27" s="34"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B28" s="34" t="s">
+        <v>212</v>
+      </c>
+      <c r="C28" s="34"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B29" s="34" t="s">
+        <v>210</v>
+      </c>
+      <c r="C29" s="34"/>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B30" s="34" t="s">
+        <v>211</v>
+      </c>
+      <c r="C30" s="34"/>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B31" s="34" t="s">
+        <v>213</v>
+      </c>
+      <c r="C31" s="34"/>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B32" s="34" t="s">
+        <v>209</v>
+      </c>
+      <c r="C32" s="34"/>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>32</v>
+      </c>
+      <c r="B33" s="34" t="s">
+        <v>216</v>
+      </c>
+      <c r="C33" s="34"/>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="B34" s="34" t="s">
+        <v>214</v>
+      </c>
+      <c r="C34" s="34"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>34</v>
+      </c>
+      <c r="B35" s="34" t="s">
+        <v>215</v>
+      </c>
+      <c r="C35" s="34"/>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="B36" s="34" t="s">
+        <v>217</v>
+      </c>
+      <c r="C36" s="34"/>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <f t="shared" si="0"/>
+        <v>36</v>
+      </c>
+      <c r="B37" s="34" t="s">
+        <v>218</v>
+      </c>
+      <c r="C37" s="34"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1621,32 +2382,77 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K20" sqref="K20"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="45.28515625" customWidth="1"/>
+    <col min="3" max="3" width="71" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B2" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B3" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="B4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="2:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="B5" s="44" t="s">
+        <v>150</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>151</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="3" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1654,136 +2460,123 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="C2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
+        <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
+        <f t="shared" ref="A4:A11" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
+        <f t="shared" si="0"/>
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
+        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>47</v>
+      </c>
+      <c r="C9" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>45</v>
-      </c>
-      <c r="C8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>46</v>
-      </c>
-      <c r="C9" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>47</v>
-      </c>
-      <c r="C10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
-      <c r="C12" t="s">
         <v>55</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" t="s">
-        <v>56</v>
       </c>
     </row>
   </sheetData>
@@ -1796,15 +2589,15 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="3" width="44.44140625" customWidth="1"/>
+    <col min="2" max="3" width="44.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1812,198 +2605,198 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+1</f>
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <f t="shared" ref="A4:A18" si="0">A3+1</f>
         <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>21</v>
+      </c>
+      <c r="C4" t="s">
         <v>22</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" s="20" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" s="20" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" s="20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
       <c r="C8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C9" t="s">
         <v>28</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="C10" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>31</v>
       </c>
-      <c r="C11" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>32</v>
       </c>
-      <c r="C12" t="s">
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>34</v>
       </c>
-      <c r="C13" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <f t="shared" si="0"/>
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>35</v>
       </c>
-      <c r="C14" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>36</v>
       </c>
-      <c r="C15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>37</v>
       </c>
-      <c r="C16" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>38</v>
       </c>
-      <c r="C17" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>39</v>
-      </c>
-      <c r="C18" t="s">
-        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -2016,49 +2809,49 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D113"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28:D31"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C63" sqref="C63:D66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.77734375" customWidth="1"/>
-    <col min="2" max="2" width="17.88671875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" style="2" customWidth="1"/>
-    <col min="4" max="4" width="68.88671875" style="2" customWidth="1"/>
+    <col min="1" max="1" width="4.7109375" customWidth="1"/>
+    <col min="2" max="2" width="17.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="68.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="C1" s="2" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="3" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="39" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="42"/>
+      <c r="D3" s="43"/>
+    </row>
+    <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="41"/>
-    </row>
-    <row r="4" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B5" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>3</v>
@@ -2067,7 +2860,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <f>A6+1</f>
         <v>2</v>
@@ -2080,13 +2873,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <f t="shared" ref="A8:A79" si="0">A7+1</f>
         <v>3</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>11</v>
@@ -2095,7 +2888,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <f t="shared" si="0"/>
         <v>4</v>
@@ -2108,7 +2901,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
@@ -2121,39 +2914,39 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B11" s="9"/>
       <c r="C11" s="3" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="D11" s="8" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B12" s="9"/>
       <c r="C12" s="3" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D12" s="8" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>7</v>
@@ -2162,7 +2955,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <f t="shared" si="0"/>
         <v>9</v>
@@ -2175,244 +2968,244 @@
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B15" s="9"/>
       <c r="C15" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B16" s="9"/>
       <c r="C16" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D16" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B17" s="9"/>
       <c r="C17" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B18" s="9"/>
       <c r="C18" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="16" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A19">
+    </row>
+    <row r="19" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="30">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="14" t="s">
+      <c r="B19" s="31"/>
+      <c r="C19" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D19" s="33" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A20" s="30">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B20" s="31"/>
+      <c r="C20" s="32" t="s">
         <v>91</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D20" s="33" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A21" s="30">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B21" s="31"/>
+      <c r="C21" s="32" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A20">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="14" t="s">
-        <v>92</v>
-      </c>
-      <c r="D20" s="15" t="s">
+      <c r="D21" s="33" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="21" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B21" s="13"/>
-      <c r="C21" s="14" t="s">
+    <row r="22" spans="1:4" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A22" s="30">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B22" s="31"/>
+      <c r="C22" s="32" t="s">
         <v>94</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D22" s="33" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A22">
-        <f t="shared" si="0"/>
-        <v>17</v>
-      </c>
-      <c r="B22" s="13"/>
-      <c r="C22" s="14" t="s">
+    <row r="23" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="30">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B23" s="31"/>
+      <c r="C23" s="32" t="s">
         <v>95</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D23" s="33" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="23" spans="1:4" s="16" customFormat="1" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A23">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B23" s="13"/>
-      <c r="C23" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="20">
+    <row r="24" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="30">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B24" s="32"/>
-      <c r="C24" s="33" t="s">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="D24" s="33" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="30">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="D25" s="33" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="D26" s="33" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="30">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B27" s="31"/>
+      <c r="C27" s="32" t="s">
         <v>172</v>
       </c>
-      <c r="D24" s="34" t="s">
+      <c r="D27" s="33" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="25" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="20">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B25" s="32"/>
-      <c r="C25" s="33" t="s">
+    <row r="28" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="30">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B28" s="31"/>
+      <c r="C28" s="32" t="s">
         <v>173</v>
       </c>
-      <c r="D25" s="34" t="s">
+      <c r="D28" s="33" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="26" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="20">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B26" s="32"/>
-      <c r="C26" s="33" t="s">
+    <row r="29" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="30">
+        <f t="shared" si="0"/>
+        <v>24</v>
+      </c>
+      <c r="B29" s="31"/>
+      <c r="C29" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="D26" s="34" t="s">
+      <c r="D29" s="33" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="27" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="20">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B27" s="32"/>
-      <c r="C27" s="33" t="s">
+    <row r="30" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="30">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="B30" s="31"/>
+      <c r="C30" s="32" t="s">
         <v>175</v>
       </c>
-      <c r="D27" s="34" t="s">
+      <c r="D30" s="33" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="28" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="20">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B28" s="32"/>
-      <c r="C28" s="33" t="s">
+    <row r="31" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="30">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B31" s="31"/>
+      <c r="C31" s="32" t="s">
         <v>176</v>
       </c>
-      <c r="D28" s="34" t="s">
+      <c r="D31" s="33" t="s">
         <v>184</v>
       </c>
     </row>
-    <row r="29" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="20">
-        <f t="shared" si="0"/>
-        <v>24</v>
-      </c>
-      <c r="B29" s="32"/>
-      <c r="C29" s="33" t="s">
-        <v>177</v>
-      </c>
-      <c r="D29" s="34" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="20">
-        <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="B30" s="32"/>
-      <c r="C30" s="33" t="s">
-        <v>178</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>186</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="35" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="20">
-        <f t="shared" si="0"/>
-        <v>26</v>
-      </c>
-      <c r="B31" s="32"/>
-      <c r="C31" s="33" t="s">
-        <v>179</v>
-      </c>
-      <c r="D31" s="34" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A32" s="20">
+    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="16">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>17</v>
       </c>
       <c r="D32" s="8" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A33" s="20">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="16">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
@@ -2421,371 +3214,371 @@
         <v>18</v>
       </c>
       <c r="D33" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A34" s="20">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="16">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
       <c r="B34" s="9"/>
       <c r="C34" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="8" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A35" s="20">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="16">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
       <c r="B35" s="9"/>
       <c r="C35" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D35" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A36" s="20">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="16">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
       <c r="B36" s="9"/>
       <c r="C36" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D36" s="8" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A37" s="20">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="16">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A38" s="20">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="16">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A39" s="20">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="16">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A40" s="20">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="16">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A41" s="20">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="16">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D41" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A42" s="20">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="16">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
       <c r="B42" s="9"/>
       <c r="C42" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D42" s="8" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A43" s="20">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="16">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
       <c r="B43" s="9"/>
       <c r="C43" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="D43" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A44" s="20">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="16">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
       <c r="B44" s="9"/>
       <c r="C44" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D44" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A45" s="20">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="16">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D45" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A46" s="20">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="16">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
       <c r="B46" s="9"/>
       <c r="C46" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D46" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A47" s="20">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A47" s="16">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
       <c r="B47" s="9"/>
       <c r="C47" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D47" s="8" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A48" s="20">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A48" s="16">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B48" s="17"/>
-      <c r="C48" s="18" t="s">
+      <c r="B48" s="13"/>
+      <c r="C48" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D48" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A49" s="16">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B49" s="13"/>
+      <c r="C49" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D49" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D48" s="19" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A49" s="20">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B49" s="17"/>
-      <c r="C49" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="D49" s="19" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A50" s="20">
+    </row>
+    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A50" s="16">
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B50" s="17"/>
-      <c r="C50" s="18" t="s">
+      <c r="B50" s="13"/>
+      <c r="C50" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="D50" s="15" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="19" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A51" s="20">
+    </row>
+    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A51" s="16">
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
       <c r="B51" s="9"/>
       <c r="C51" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D51" s="8" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A52" s="20">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A52" s="16">
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
       <c r="B52" s="9"/>
       <c r="C52" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D52" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="D52" s="8" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A53" s="20">
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="16">
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
       <c r="B53" s="9"/>
       <c r="C53" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D53" s="8"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A54" s="20">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="16">
         <f t="shared" si="0"/>
         <v>49</v>
       </c>
       <c r="B54" s="9"/>
       <c r="C54" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D54" s="8"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A55" s="20">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="16">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
       <c r="B55" s="9"/>
       <c r="C55" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D55" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="D55" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A56" s="20">
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="16">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
       <c r="B56" s="9"/>
       <c r="C56" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D56" s="8"/>
     </row>
-    <row r="57" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A57" s="20">
+    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A57" s="16">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
       <c r="B57" s="9"/>
       <c r="C57" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D57" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A58" s="20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A58" s="16">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
       <c r="B58" s="9"/>
       <c r="C58" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D58" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A59" s="20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="16">
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
       <c r="B59" s="9"/>
       <c r="C59" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D59" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A60" s="20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A60" s="16">
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
       <c r="B60" s="9"/>
       <c r="C60" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D60" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A61" s="20">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A61" s="16">
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
       <c r="B61" s="9"/>
       <c r="C61" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D61" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="D61" s="8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A62" s="20">
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="16">
         <f t="shared" si="0"/>
         <v>57</v>
       </c>
@@ -2793,396 +3586,396 @@
       <c r="C62" s="3"/>
       <c r="D62" s="8"/>
     </row>
-    <row r="63" spans="1:4" ht="29.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A63" s="20">
+    <row r="63" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="16">
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
       <c r="B63" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C63" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>76</v>
-      </c>
       <c r="D63" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A64" s="20">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="16">
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
       <c r="B64" s="9"/>
       <c r="C64" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D64" s="8" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="43.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A65" s="20">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="16">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
       <c r="B65" s="10"/>
       <c r="C65" s="11" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D65" s="12" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" s="24" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A66" s="20">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" s="20" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="16">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B66" s="28"/>
-      <c r="C66" s="29" t="s">
-        <v>153</v>
-      </c>
-      <c r="D66" s="30" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A67" s="20">
+      <c r="B66" s="24"/>
+      <c r="C66" s="25" t="s">
+        <v>150</v>
+      </c>
+      <c r="D66" s="26" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="16">
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B67" s="27" t="s">
-        <v>134</v>
-      </c>
-      <c r="C67" s="24" t="s">
-        <v>151</v>
-      </c>
-      <c r="D67" s="22" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A68" s="20">
+      <c r="B67" s="23" t="s">
+        <v>131</v>
+      </c>
+      <c r="C67" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="D67" s="18" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="16">
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B68" s="22"/>
-      <c r="C68" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="D68" s="22" t="s">
+      <c r="B68" s="18"/>
+      <c r="C68" s="20" t="s">
+        <v>147</v>
+      </c>
+      <c r="D68" s="18" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="16">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="C69" s="18" t="s">
         <v>135</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A69" s="20">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="C69" s="22" t="s">
+      <c r="D69" s="18" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="16">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="C70" s="18" t="s">
+        <v>136</v>
+      </c>
+      <c r="D70" s="18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="16">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="C71" s="18" t="s">
+        <v>137</v>
+      </c>
+      <c r="D71" s="18" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="16">
+        <f t="shared" si="0"/>
+        <v>67</v>
+      </c>
+      <c r="C72" s="18" t="s">
         <v>138</v>
       </c>
-      <c r="D69" s="22" t="s">
+      <c r="D72" s="18" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A70" s="20">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="C70" s="22" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="16">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+      <c r="C73" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="D70" s="22" t="s">
+      <c r="D73" s="18" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A71" s="20">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="C71" s="22" t="s">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="16">
+        <f t="shared" si="0"/>
+        <v>69</v>
+      </c>
+      <c r="C74" s="18" t="s">
         <v>140</v>
       </c>
-      <c r="D71" s="22" t="s">
+      <c r="D74" s="18" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A72" s="20">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="C72" s="22" t="s">
-        <v>141</v>
-      </c>
-      <c r="D72" s="22" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A73" s="20">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="C73" s="22" t="s">
-        <v>142</v>
-      </c>
-      <c r="D73" s="22" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A74" s="20">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="C74" s="22" t="s">
-        <v>143</v>
-      </c>
-      <c r="D74" s="22" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A75" s="20">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="16">
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="C75" s="22" t="s">
-        <v>159</v>
-      </c>
-      <c r="D75" s="22" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A76" s="20">
+      <c r="C75" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="D75" s="18" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="16">
         <f t="shared" si="0"/>
         <v>71</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A77" s="20">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="16">
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A78" s="20">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="16">
         <f t="shared" si="0"/>
         <v>73</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A79" s="20">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="16">
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A80" s="20">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="16">
         <f t="shared" ref="A80:A113" si="1">A79+1</f>
         <v>75</v>
       </c>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A81" s="20">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="16">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A82" s="20">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="16">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A83" s="20">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="16">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A84" s="20">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="16">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A85" s="20">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A85" s="16">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A86" s="20">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="16">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A87" s="20">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="16">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A88" s="20">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A88" s="16">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A89" s="20">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="16">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A90" s="20">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A90" s="16">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A91" s="20">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A91" s="16">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A92" s="20">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A92" s="16">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A93" s="20">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="16">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A94" s="20">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A94" s="16">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A95" s="20">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A95" s="16">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A96" s="20">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A96" s="16">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A97" s="20">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="16">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A98" s="20">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A98" s="16">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A99" s="20">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A99" s="16">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A100" s="20">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A100" s="16">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A101" s="20">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A101" s="16">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A102" s="20">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A102" s="16">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A103" s="20">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A103" s="16">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A104" s="20">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A104" s="16">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A105" s="20">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A105" s="16">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A106" s="20">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A106" s="16">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A107" s="20">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A107" s="16">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A108" s="20">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A108" s="16">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A109" s="20">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A109" s="16">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A110" s="20">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A110" s="16">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A111" s="20">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A111" s="16">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A112" s="20">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A112" s="16">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A113" s="20">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A113" s="16">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
@@ -3198,208 +3991,263 @@
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C17"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.44140625" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" customWidth="1"/>
-    <col min="3" max="3" width="53.33203125" customWidth="1"/>
+    <col min="1" max="1" width="4.42578125" customWidth="1"/>
+    <col min="2" max="2" width="50.85546875" customWidth="1"/>
+    <col min="3" max="3" width="53.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>169</v>
-      </c>
-      <c r="B1" s="31" t="s">
-        <v>170</v>
-      </c>
-      <c r="C1" s="31" t="s">
-        <v>171</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B1" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="C1" s="27" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C2" s="17" t="s">
         <v>112</v>
       </c>
-      <c r="C2" s="21" t="s">
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <f>A2+1</f>
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>110</v>
+      </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <f t="shared" ref="A4:A20" si="0">A3+1</f>
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>113</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
-        <v>113</v>
-      </c>
-      <c r="C3" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="C5" t="s">
         <v>116</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>117</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>118</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C7" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>120</v>
       </c>
-      <c r="C6" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="C8" t="s">
         <v>121</v>
       </c>
-      <c r="C7" t="s">
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>122</v>
       </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="C9" t="s">
         <v>123</v>
       </c>
-      <c r="C8" t="s">
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+      <c r="C10" t="s">
         <v>125</v>
       </c>
-      <c r="C9" t="s">
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="22" t="s">
         <v>126</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+      <c r="C11" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C10" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="25">
-        <v>10</v>
-      </c>
-      <c r="B11" s="26" t="s">
+    </row>
+    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="21" t="s">
         <v>129</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C12" s="19" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="25">
-        <v>11</v>
-      </c>
-      <c r="B12" s="25" t="s">
-        <v>132</v>
-      </c>
-      <c r="C12" s="23" t="s">
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>12</v>
+      </c>
+      <c r="B13" s="22" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="13" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A13" s="25">
-        <v>12</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>136</v>
-      </c>
-      <c r="C13" s="23" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="24" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="25">
+      <c r="C13" s="19" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="24" t="s">
+      <c r="B14" s="20" t="s">
+        <v>152</v>
+      </c>
+      <c r="C14" s="20" t="s">
         <v>155</v>
       </c>
-      <c r="C14" s="24" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="24" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="25">
+    </row>
+    <row r="15" spans="1:3" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="25" t="s">
-        <v>156</v>
-      </c>
-      <c r="C15" s="23" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="25">
+      <c r="B15" s="21" t="s">
+        <v>153</v>
+      </c>
+      <c r="C15" s="19" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="25" t="s">
+      <c r="B16" s="21" t="s">
+        <v>162</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="21" t="s">
+        <v>164</v>
+      </c>
+      <c r="C17" s="22" t="s">
         <v>165</v>
       </c>
-      <c r="C16" s="25" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="A17" s="25">
-        <v>16</v>
-      </c>
-      <c r="B17" s="25" t="s">
-        <v>167</v>
-      </c>
-      <c r="C17" s="26" t="s">
-        <v>168</v>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="B18" s="21" t="s">
+        <v>245</v>
+      </c>
+      <c r="C18" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="21" t="s">
+        <v>244</v>
+      </c>
+      <c r="C19" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B20" s="21" t="s">
+        <v>246</v>
+      </c>
+      <c r="C20" t="s">
+        <v>247</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B19" r:id="rId1" tooltip="Tutorial_softRealTimeJointsVelControl.m" display="https://github.com/Modi1987/KST-Kuka-Sunrise-Toolbox/blob/master/Matlab_Client1.6/Tutorial_softRealTimeJointsVelControl.m"/>
+    <hyperlink ref="B18" r:id="rId2" tooltip="Tutorial_realTimeImpedencePlotTorqueFeedBack.m" display="https://github.com/Modi1987/KST-Kuka-Sunrise-Toolbox/blob/master/Matlab_Client1.6/Tutorial_realTimeImpedencePlotTorqueFeedBack.m"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Total list of functions is established
</commit_message>
<xml_diff>
--- a/Toolbox function.xlsx
+++ b/Toolbox function.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11385" windowHeight="10125" tabRatio="944" activeTab="8"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11730" tabRatio="944" activeTab="7"/>
   </bookViews>
   <sheets>
     <sheet name="about" sheetId="3" r:id="rId1"/>
@@ -16,14 +16,13 @@
     <sheet name="read parameters" sheetId="4" r:id="rId7"/>
     <sheet name="TLM" sheetId="9" r:id="rId8"/>
     <sheet name="exmple files" sheetId="7" r:id="rId9"/>
-    <sheet name="Sheet1" sheetId="10" r:id="rId10"/>
   </sheets>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="250">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="436" uniqueCount="256">
   <si>
     <t>method</t>
   </si>
@@ -236,9 +235,6 @@
 motion control</t>
   </si>
   <si>
-    <t>TLM total list of supported functions</t>
-  </si>
-  <si>
     <t>Setters</t>
   </si>
   <si>
@@ -695,9 +691,6 @@
     <t>sendEEfPositionf</t>
   </si>
   <si>
-    <t>net_pinIIWA</t>
-  </si>
-  <si>
     <t>Ping the controller</t>
   </si>
   <si>
@@ -737,12 +730,6 @@
     <t>Send distnination position for joints angles to the robot,</t>
   </si>
   <si>
-    <t>start the soft real time control in joint velocity mod</t>
-  </si>
-  <si>
-    <t>stop the soft real time control in joint velocity mod</t>
-  </si>
-  <si>
     <t>Send reference velocities for joints of the robot,</t>
   </si>
   <si>
@@ -774,13 +761,43 @@
   </si>
   <si>
     <t>´Realtime control using joint space velocity control mode</t>
+  </si>
+  <si>
+    <t>net_pingIIWA</t>
+  </si>
+  <si>
+    <t>moveWaitForDTWhenInterrupted.m</t>
+  </si>
+  <si>
+    <t>Peform linear motion of EEF, this motion  is interrptible, this happens when the joints torques exceed a predefiend limit, causing the robot to stop its motion In such a case, the robot stops in place when a collision is detected, and awaits for double touch from the coworker for it to resume its operation. The motion can be interrupted and resumed several times in a single call. The funtion is blocking, and it returns when the distination is reached.</t>
+  </si>
+  <si>
+    <t>start the soft real time control in joint velocity mode</t>
+  </si>
+  <si>
+    <t>stop the soft real time control in joint velocity mode</t>
+  </si>
+  <si>
+    <t>gen_NullSpaceMatrix</t>
+  </si>
+  <si>
+    <t>calculates the null space projection matrix</t>
+  </si>
+  <si>
+    <t>start the direct servo for real time control, cartesian space.</t>
+  </si>
+  <si>
+    <t>stop the direct servo for real time control, cartesian space.</t>
+  </si>
+  <si>
+    <t>Total List of Methods (TLM)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -829,6 +846,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="20"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1049,25 +1083,10 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1080,16 +1099,28 @@
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1135,31 +1166,10 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1188,6 +1198,28 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1206,11 +1238,59 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1523,17 +1603,17 @@
   <sheetData>
     <row r="1" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="38" t="s">
+      <c r="B2" s="39" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="40"/>
+      <c r="C2" s="40"/>
+      <c r="D2" s="40"/>
+      <c r="E2" s="40"/>
+      <c r="F2" s="40"/>
+      <c r="G2" s="40"/>
+      <c r="H2" s="40"/>
+      <c r="I2" s="40"/>
+      <c r="J2" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1544,26 +1624,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A5" sqref="A4:XFD5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1583,10 +1649,10 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="25" t="s">
         <v>4</v>
       </c>
     </row>
@@ -1595,10 +1661,10 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="25" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1607,22 +1673,22 @@
         <f>A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="C4" s="25" t="s">
         <v>198</v>
-      </c>
-      <c r="C4" s="32" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="32" t="s">
-        <v>223</v>
-      </c>
-      <c r="C5" s="32" t="s">
-        <v>224</v>
+      <c r="B5" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -1635,7 +1701,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:C1"/>
+      <selection activeCell="B27" sqref="B2:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1656,7 +1722,7 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="25" t="s">
         <v>11</v>
       </c>
       <c r="C2" s="3" t="s">
@@ -1668,7 +1734,7 @@
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="25" t="s">
         <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
@@ -1680,7 +1746,7 @@
         <f t="shared" ref="A4:A27" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="25" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="3" t="s">
@@ -1693,10 +1759,10 @@
         <v>4</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1705,10 +1771,10 @@
         <v>5</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1716,8 +1782,8 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="32" t="s">
-        <v>219</v>
+      <c r="B7" s="25" t="s">
+        <v>218</v>
       </c>
       <c r="C7" s="3"/>
     </row>
@@ -1726,8 +1792,8 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>220</v>
+      <c r="B8" s="25" t="s">
+        <v>219</v>
       </c>
       <c r="C8" s="3"/>
     </row>
@@ -1736,11 +1802,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="32" t="s">
+      <c r="B9" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1748,11 +1814,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>89</v>
+      <c r="B10" s="25" t="s">
+        <v>88</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1760,8 +1826,8 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="32" t="s">
-        <v>221</v>
+      <c r="B11" s="25" t="s">
+        <v>220</v>
       </c>
       <c r="C11" s="3"/>
     </row>
@@ -1770,8 +1836,8 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>222</v>
+      <c r="B12" s="25" t="s">
+        <v>221</v>
       </c>
       <c r="C12" s="3"/>
     </row>
@@ -1780,11 +1846,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="28" t="s">
-        <v>185</v>
-      </c>
-      <c r="C13" s="29" t="s">
-        <v>189</v>
+      <c r="B13" s="21" t="s">
+        <v>184</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>188</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1792,11 +1858,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="28" t="s">
-        <v>186</v>
-      </c>
-      <c r="C14" s="29" t="s">
-        <v>190</v>
+      <c r="B14" s="21" t="s">
+        <v>185</v>
+      </c>
+      <c r="C14" s="22" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1804,11 +1870,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="28" t="s">
-        <v>187</v>
-      </c>
-      <c r="C15" s="29" t="s">
-        <v>191</v>
+      <c r="B15" s="21" t="s">
+        <v>186</v>
+      </c>
+      <c r="C15" s="22" t="s">
+        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1816,11 +1882,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="28" t="s">
-        <v>188</v>
-      </c>
-      <c r="C16" s="29" t="s">
-        <v>192</v>
+      <c r="B16" s="21" t="s">
+        <v>187</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>191</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1828,11 +1894,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="36" t="s">
-        <v>196</v>
-      </c>
-      <c r="C17" s="37" t="s">
-        <v>232</v>
+      <c r="B17" s="29" t="s">
+        <v>195</v>
+      </c>
+      <c r="C17" s="30" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1840,11 +1906,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="36" t="s">
-        <v>193</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>233</v>
+      <c r="B18" s="29" t="s">
+        <v>192</v>
+      </c>
+      <c r="C18" s="30" t="s">
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1852,11 +1918,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="36" t="s">
-        <v>194</v>
-      </c>
-      <c r="C19" s="37" t="s">
-        <v>234</v>
+      <c r="B19" s="29" t="s">
+        <v>193</v>
+      </c>
+      <c r="C19" s="30" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1864,11 +1930,11 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="36" t="s">
-        <v>195</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>235</v>
+      <c r="B20" s="29" t="s">
+        <v>194</v>
+      </c>
+      <c r="C20" s="30" t="s">
+        <v>233</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1876,11 +1942,11 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="34" t="s">
-        <v>225</v>
+      <c r="B21" s="27" t="s">
+        <v>223</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>237</v>
+        <v>249</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1888,11 +1954,11 @@
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="34" t="s">
-        <v>226</v>
+      <c r="B22" s="27" t="s">
+        <v>224</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>238</v>
+        <v>250</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1900,11 +1966,11 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="34" t="s">
-        <v>227</v>
+      <c r="B23" s="27" t="s">
+        <v>225</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1912,11 +1978,11 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="34" t="s">
-        <v>228</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>240</v>
+      <c r="B24" s="27" t="s">
+        <v>226</v>
+      </c>
+      <c r="C24" s="21" t="s">
+        <v>236</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1924,11 +1990,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="34" t="s">
-        <v>229</v>
-      </c>
-      <c r="C25" s="28" t="s">
-        <v>241</v>
+      <c r="B25" s="27" t="s">
+        <v>227</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>237</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1936,11 +2002,11 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="34" t="s">
-        <v>230</v>
-      </c>
-      <c r="C26" s="28" t="s">
-        <v>242</v>
+      <c r="B26" s="27" t="s">
+        <v>228</v>
+      </c>
+      <c r="C26" s="21" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -1948,11 +2014,11 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="34" t="s">
-        <v>231</v>
-      </c>
-      <c r="C27" s="28" t="s">
-        <v>243</v>
+      <c r="B27" s="27" t="s">
+        <v>229</v>
+      </c>
+      <c r="C27" s="21" t="s">
+        <v>239</v>
       </c>
     </row>
   </sheetData>
@@ -1964,8 +2030,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C37"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="B43" sqref="B43"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1975,10 +2041,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="35" t="s">
+      <c r="C1" s="28" t="s">
         <v>1</v>
       </c>
     </row>
@@ -1986,10 +2052,10 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="32" t="s">
+      <c r="C2" s="25" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1998,10 +2064,10 @@
         <f>1+A2</f>
         <v>2</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="32" t="s">
+      <c r="C3" s="25" t="s">
         <v>10</v>
       </c>
     </row>
@@ -2010,10 +2076,10 @@
         <f t="shared" ref="A4:A37" si="0">1+A3</f>
         <v>3</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C4" s="32" t="s">
+      <c r="C4" s="25" t="s">
         <v>63</v>
       </c>
     </row>
@@ -2022,10 +2088,10 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="25" t="s">
         <v>62</v>
       </c>
     </row>
@@ -2034,11 +2100,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="C6" s="32" t="s">
-        <v>92</v>
+      <c r="B6" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="C6" s="25" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2046,11 +2112,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="C7" s="32" t="s">
-        <v>96</v>
+      <c r="B7" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="25" t="s">
+        <v>95</v>
       </c>
     </row>
     <row r="8" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2058,11 +2124,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="C8" s="32" t="s">
-        <v>97</v>
+      <c r="B8" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="C8" s="25" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2070,11 +2136,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="C9" s="32" t="s">
-        <v>98</v>
+      <c r="B9" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="C9" s="25" t="s">
+        <v>97</v>
       </c>
     </row>
     <row r="10" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -2082,11 +2148,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B10" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>99</v>
+      <c r="B10" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="C10" s="25" t="s">
+        <v>98</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2094,11 +2160,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B11" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="C11" s="32" t="s">
-        <v>177</v>
+      <c r="B11" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="C11" s="25" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2106,11 +2172,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="C12" s="32" t="s">
-        <v>178</v>
+      <c r="B12" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="C12" s="25" t="s">
+        <v>177</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2118,11 +2184,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="C13" s="32" t="s">
-        <v>179</v>
+      <c r="B13" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="C13" s="25" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2130,11 +2196,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="C14" s="32" t="s">
-        <v>180</v>
+      <c r="B14" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="C14" s="25" t="s">
+        <v>179</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2142,11 +2208,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B15" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="C15" s="32" t="s">
-        <v>181</v>
+      <c r="B15" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="C15" s="25" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2154,11 +2220,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="C16" s="32" t="s">
-        <v>182</v>
+      <c r="B16" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="C16" s="25" t="s">
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2166,11 +2232,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B17" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="C17" s="32" t="s">
-        <v>183</v>
+      <c r="B17" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="C17" s="25" t="s">
+        <v>182</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -2178,11 +2244,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="C18" s="32" t="s">
-        <v>184</v>
+      <c r="B18" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="C18" s="25" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -2190,190 +2256,190 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B19" s="34" t="s">
-        <v>200</v>
-      </c>
-      <c r="C19" s="34"/>
+      <c r="B19" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="C19" s="27"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="34" t="s">
-        <v>202</v>
-      </c>
-      <c r="C20" s="34"/>
+      <c r="B20" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="C20" s="27"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B21" s="34" t="s">
-        <v>203</v>
-      </c>
-      <c r="C21" s="34"/>
+      <c r="B21" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="C21" s="27"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B22" s="34" t="s">
-        <v>204</v>
-      </c>
-      <c r="C22" s="34"/>
+      <c r="B22" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="C22" s="27"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B23" s="34" t="s">
-        <v>205</v>
-      </c>
-      <c r="C23" s="34"/>
+      <c r="B23" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="C23" s="27"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B24" s="34" t="s">
-        <v>206</v>
-      </c>
-      <c r="C24" s="34"/>
+      <c r="B24" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="27"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B25" s="34" t="s">
-        <v>207</v>
-      </c>
-      <c r="C25" s="34"/>
+      <c r="B25" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="C25" s="27"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B26" s="34" t="s">
-        <v>208</v>
-      </c>
-      <c r="C26" s="34"/>
+      <c r="B26" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="C26" s="27"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B27" s="34" t="s">
-        <v>201</v>
-      </c>
-      <c r="C27" s="34"/>
+      <c r="B27" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="C27" s="27"/>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B28" s="34" t="s">
-        <v>212</v>
-      </c>
-      <c r="C28" s="34"/>
+      <c r="B28" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="C28" s="27"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B29" s="34" t="s">
-        <v>210</v>
-      </c>
-      <c r="C29" s="34"/>
+      <c r="B29" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="C29" s="27"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B30" s="34" t="s">
-        <v>211</v>
-      </c>
-      <c r="C30" s="34"/>
+      <c r="B30" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="C30" s="27"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B31" s="34" t="s">
-        <v>213</v>
-      </c>
-      <c r="C31" s="34"/>
+      <c r="B31" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="C31" s="27"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B32" s="34" t="s">
-        <v>209</v>
-      </c>
-      <c r="C32" s="34"/>
+      <c r="B32" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="C32" s="27"/>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B33" s="34" t="s">
-        <v>216</v>
-      </c>
-      <c r="C33" s="34"/>
+      <c r="B33" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="C33" s="27"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B34" s="34" t="s">
-        <v>214</v>
-      </c>
-      <c r="C34" s="34"/>
+      <c r="B34" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="C34" s="27"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B35" s="34" t="s">
-        <v>215</v>
-      </c>
-      <c r="C35" s="34"/>
+      <c r="B35" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="C35" s="27"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B36" s="34" t="s">
-        <v>217</v>
-      </c>
-      <c r="C36" s="34"/>
+      <c r="B36" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="C36" s="27"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B37" s="34" t="s">
-        <v>218</v>
-      </c>
-      <c r="C37" s="34"/>
+      <c r="B37" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="C37" s="27"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2382,10 +2448,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:C5"/>
+  <dimension ref="B1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2404,38 +2470,50 @@
     </row>
     <row r="2" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B2" s="3" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B3" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="2:3" ht="45" x14ac:dyDescent="0.25">
       <c r="B4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="5" spans="2:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="B5" s="44" t="s">
+      <c r="B5" s="31" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="31" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="44" t="s">
-        <v>151</v>
+    </row>
+    <row r="6" spans="2:3" ht="90" x14ac:dyDescent="0.25">
+      <c r="B6" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="C6" s="38" t="s">
+        <v>248</v>
       </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B6" r:id="rId1" tooltip="moveWaitForDTWhenInterrupted.m" display="https://github.com/Modi1987/KST-Kuka-Sunrise-Toolbox/blob/master/Matlab_Client1.6/moveWaitForDTWhenInterrupted.m"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>
 </file>
 
@@ -2646,7 +2724,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="16" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -2655,7 +2733,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -2664,7 +2742,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="16" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -2700,7 +2778,7 @@
         <v>29</v>
       </c>
       <c r="C10" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -2712,7 +2790,7 @@
         <v>30</v>
       </c>
       <c r="C11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -2736,7 +2814,7 @@
         <v>33</v>
       </c>
       <c r="C13" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -2807,32 +2885,34 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D113"/>
+  <dimension ref="A1:D155"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C63" sqref="C63:D66"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.7109375" customWidth="1"/>
     <col min="2" max="2" width="17.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="58" style="2" customWidth="1"/>
     <col min="4" max="4" width="68.85546875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C1" s="2" t="s">
-        <v>70</v>
-      </c>
+    <row r="1" spans="1:4" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B1" s="60" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="61"/>
+      <c r="D1" s="62"/>
     </row>
     <row r="2" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="3" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="41" t="s">
+      <c r="B3" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="C3" s="42"/>
-      <c r="D3" s="43"/>
+      <c r="C3" s="43"/>
+      <c r="D3" s="44"/>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -2853,10 +2933,10 @@
       <c r="B6" s="7" t="s">
         <v>68</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="48" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="49" t="s">
         <v>4</v>
       </c>
     </row>
@@ -2873,19 +2953,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" ref="A8:A79" si="0">A7+1</f>
+        <f t="shared" ref="A8:A71" si="0">A7+1</f>
         <v>3</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>16</v>
+      <c r="B8" s="25"/>
+      <c r="C8" s="25" t="s">
+        <v>197</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
@@ -2893,25 +2971,27 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B9" s="9"/>
-      <c r="C9" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B9" s="25"/>
+      <c r="C9" s="25" t="s">
+        <v>246</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B10" s="9"/>
-      <c r="C10" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="8" t="s">
-        <v>15</v>
+      <c r="B10" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="48" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
@@ -2920,11 +3000,11 @@
         <v>6</v>
       </c>
       <c r="B11" s="9"/>
-      <c r="C11" s="3" t="s">
-        <v>158</v>
-      </c>
-      <c r="D11" s="8" t="s">
-        <v>160</v>
+      <c r="C11" s="25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -2933,26 +3013,24 @@
         <v>7</v>
       </c>
       <c r="B12" s="9"/>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B13" s="9"/>
+      <c r="C13" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="D13" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B13" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C13" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D13" s="8" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -2962,1027 +3040,1441 @@
       </c>
       <c r="B14" s="9"/>
       <c r="C14" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D14" s="8" t="s">
+        <v>158</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B15" s="9"/>
-      <c r="C15" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="D15" s="8" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B15" s="24"/>
+      <c r="C15" s="25" t="s">
+        <v>218</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B16" s="9"/>
-      <c r="C16" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="D16" s="8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B16" s="24"/>
+      <c r="C16" s="25" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="A17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B17" s="9"/>
-      <c r="C17" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B17" s="24"/>
+      <c r="C17" s="25" t="s">
+        <v>18</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B18" s="9"/>
-      <c r="C18" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="30">
+      <c r="B18" s="24"/>
+      <c r="C18" s="25" t="s">
+        <v>88</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B19" s="31"/>
-      <c r="C19" s="32" t="s">
-        <v>90</v>
-      </c>
-      <c r="D19" s="33" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="30">
+      <c r="B19" s="24"/>
+      <c r="C19" s="25" t="s">
+        <v>220</v>
+      </c>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A20">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B20" s="31"/>
-      <c r="C20" s="32" t="s">
-        <v>91</v>
-      </c>
-      <c r="D20" s="33" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A21" s="30">
+      <c r="B20" s="24"/>
+      <c r="C20" s="25" t="s">
+        <v>221</v>
+      </c>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21">
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B21" s="31"/>
-      <c r="C21" s="32" t="s">
-        <v>93</v>
-      </c>
-      <c r="D21" s="33" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" s="30" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="30">
+      <c r="B21" s="24"/>
+      <c r="C21" s="55" t="s">
+        <v>184</v>
+      </c>
+      <c r="D21" s="56" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B22" s="31"/>
-      <c r="C22" s="32" t="s">
-        <v>94</v>
-      </c>
-      <c r="D22" s="33" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="30">
+      <c r="B22" s="24"/>
+      <c r="C22" s="55" t="s">
+        <v>185</v>
+      </c>
+      <c r="D22" s="56" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B23" s="31"/>
-      <c r="C23" s="32" t="s">
-        <v>95</v>
-      </c>
-      <c r="D23" s="33" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="30">
+      <c r="B23" s="24"/>
+      <c r="C23" s="55" t="s">
+        <v>186</v>
+      </c>
+      <c r="D23" s="56" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B24" s="31"/>
-      <c r="C24" s="32" t="s">
-        <v>169</v>
-      </c>
-      <c r="D24" s="33" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="30">
+      <c r="B24" s="24"/>
+      <c r="C24" s="55" t="s">
+        <v>187</v>
+      </c>
+      <c r="D24" s="56" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25">
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B25" s="31"/>
-      <c r="C25" s="32" t="s">
-        <v>170</v>
-      </c>
-      <c r="D25" s="33" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="30">
+      <c r="B25" s="24"/>
+      <c r="C25" s="57" t="s">
+        <v>195</v>
+      </c>
+      <c r="D25" s="58" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26">
         <f t="shared" si="0"/>
         <v>21</v>
       </c>
-      <c r="B26" s="31"/>
-      <c r="C26" s="32" t="s">
-        <v>171</v>
-      </c>
-      <c r="D26" s="33" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="30">
+      <c r="B26" s="24"/>
+      <c r="C26" s="57" t="s">
+        <v>192</v>
+      </c>
+      <c r="D26" s="58" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27">
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B27" s="31"/>
-      <c r="C27" s="32" t="s">
-        <v>172</v>
-      </c>
-      <c r="D27" s="33" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" s="30" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="30">
+      <c r="B27" s="24"/>
+      <c r="C27" s="57" t="s">
+        <v>193</v>
+      </c>
+      <c r="D27" s="58" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28">
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B28" s="31"/>
-      <c r="C28" s="32" t="s">
-        <v>173</v>
-      </c>
-      <c r="D28" s="33" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="30">
+      <c r="B28" s="24"/>
+      <c r="C28" s="57" t="s">
+        <v>194</v>
+      </c>
+      <c r="D28" s="58" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A29">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B29" s="31"/>
-      <c r="C29" s="32" t="s">
-        <v>174</v>
-      </c>
-      <c r="D29" s="33" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A30" s="30">
+      <c r="B29" s="24"/>
+      <c r="C29" s="59" t="s">
+        <v>223</v>
+      </c>
+      <c r="D29" s="38" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A30">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B30" s="31"/>
-      <c r="C30" s="32" t="s">
-        <v>175</v>
-      </c>
-      <c r="D30" s="33" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="30" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="A31" s="30">
+      <c r="B30" s="24"/>
+      <c r="C30" s="59" t="s">
+        <v>224</v>
+      </c>
+      <c r="D30" s="38" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A31">
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B31" s="31"/>
-      <c r="C31" s="32" t="s">
-        <v>176</v>
-      </c>
-      <c r="D31" s="33" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="16">
+      <c r="B31" s="24"/>
+      <c r="C31" s="59" t="s">
+        <v>225</v>
+      </c>
+      <c r="D31" s="38" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32">
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B32" s="7" t="s">
+      <c r="B32" s="24"/>
+      <c r="C32" s="59" t="s">
+        <v>226</v>
+      </c>
+      <c r="D32" s="55" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <f t="shared" si="0"/>
+        <v>28</v>
+      </c>
+      <c r="B33" s="24"/>
+      <c r="C33" s="59" t="s">
+        <v>227</v>
+      </c>
+      <c r="D33" s="55" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B34" s="24"/>
+      <c r="C34" s="59" t="s">
+        <v>228</v>
+      </c>
+      <c r="D34" s="55" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B35" s="24"/>
+      <c r="C35" s="59" t="s">
+        <v>229</v>
+      </c>
+      <c r="D35" s="55" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B36" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="C32" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D32" s="8" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="16">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B33" s="9"/>
-      <c r="C33" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D33" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="16">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B34" s="9"/>
-      <c r="C34" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="D34" s="8" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="16">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B35" s="9"/>
-      <c r="C35" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="16">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B36" s="9"/>
-      <c r="C36" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="D36" s="8" t="s">
-        <v>51</v>
+      <c r="C36" s="48" t="s">
+        <v>7</v>
+      </c>
+      <c r="D36" s="49" t="s">
+        <v>9</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="16">
+      <c r="A37">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
       <c r="B37" s="9"/>
       <c r="C37" s="3" t="s">
-        <v>42</v>
+        <v>8</v>
       </c>
       <c r="D37" s="8" t="s">
-        <v>52</v>
+        <v>10</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="16">
+      <c r="A38">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="3" t="s">
-        <v>43</v>
+        <v>60</v>
       </c>
       <c r="D38" s="8" t="s">
-        <v>53</v>
+        <v>63</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="16">
+      <c r="A39">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
       <c r="B39" s="9"/>
       <c r="C39" s="3" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="D39" s="8" t="s">
-        <v>59</v>
+        <v>85</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="16">
+      <c r="A40">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
       <c r="B40" s="9"/>
       <c r="C40" s="3" t="s">
-        <v>45</v>
+        <v>84</v>
       </c>
       <c r="D40" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" s="16">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
       <c r="B41" s="9"/>
       <c r="C41" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="D41" s="8" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="B42" s="24"/>
+      <c r="C42" s="25" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="26" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A43">
+        <f t="shared" si="0"/>
+        <v>38</v>
+      </c>
+      <c r="B43" s="24"/>
+      <c r="C43" s="25" t="s">
+        <v>90</v>
+      </c>
+      <c r="D43" s="26" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A44">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="B44" s="24"/>
+      <c r="C44" s="25" t="s">
+        <v>92</v>
+      </c>
+      <c r="D44" s="26" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" s="23" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+      <c r="A45">
+        <f t="shared" si="0"/>
+        <v>40</v>
+      </c>
+      <c r="B45" s="24"/>
+      <c r="C45" s="25" t="s">
+        <v>93</v>
+      </c>
+      <c r="D45" s="26" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="B46" s="24"/>
+      <c r="C46" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="D46" s="26" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47">
+        <f t="shared" si="0"/>
+        <v>42</v>
+      </c>
+      <c r="B47" s="24"/>
+      <c r="C47" s="25" t="s">
+        <v>168</v>
+      </c>
+      <c r="D47" s="26" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="B48" s="24"/>
+      <c r="C48" s="25" t="s">
+        <v>169</v>
+      </c>
+      <c r="D48" s="26" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B49" s="24"/>
+      <c r="C49" s="25" t="s">
+        <v>170</v>
+      </c>
+      <c r="D49" s="26" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B50" s="24"/>
+      <c r="C50" s="25" t="s">
+        <v>171</v>
+      </c>
+      <c r="D50" s="26" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51">
+        <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="D41" s="8" t="s">
+      <c r="B51" s="24"/>
+      <c r="C51" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="D51" s="26" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A52">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B52" s="24"/>
+      <c r="C52" s="25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" s="26" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B53" s="24"/>
+      <c r="C53" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="D53" s="26" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" s="23" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="A54">
+        <f t="shared" si="0"/>
+        <v>49</v>
+      </c>
+      <c r="B54" s="24"/>
+      <c r="C54" s="25" t="s">
+        <v>175</v>
+      </c>
+      <c r="D54" s="26" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A55">
+        <f t="shared" si="0"/>
+        <v>50</v>
+      </c>
+      <c r="B55" s="24"/>
+      <c r="C55" s="27" t="s">
+        <v>199</v>
+      </c>
+      <c r="D55" s="27"/>
+    </row>
+    <row r="56" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A56">
+        <f t="shared" si="0"/>
+        <v>51</v>
+      </c>
+      <c r="B56" s="24"/>
+      <c r="C56" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="D56" s="27"/>
+    </row>
+    <row r="57" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A57">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="B57" s="24"/>
+      <c r="C57" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="D57" s="27"/>
+    </row>
+    <row r="58" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A58">
+        <f t="shared" si="0"/>
+        <v>53</v>
+      </c>
+      <c r="B58" s="24"/>
+      <c r="C58" s="27" t="s">
+        <v>203</v>
+      </c>
+      <c r="D58" s="27"/>
+    </row>
+    <row r="59" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A59">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B59" s="24"/>
+      <c r="C59" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="D59" s="27"/>
+    </row>
+    <row r="60" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A60">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B60" s="24"/>
+      <c r="C60" s="27" t="s">
+        <v>205</v>
+      </c>
+      <c r="D60" s="27"/>
+    </row>
+    <row r="61" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A61">
+        <f t="shared" si="0"/>
+        <v>56</v>
+      </c>
+      <c r="B61" s="24"/>
+      <c r="C61" s="27" t="s">
+        <v>206</v>
+      </c>
+      <c r="D61" s="27"/>
+    </row>
+    <row r="62" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62">
+        <f t="shared" si="0"/>
         <v>57</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="16">
-        <f t="shared" si="0"/>
-        <v>37</v>
-      </c>
-      <c r="B42" s="9"/>
-      <c r="C42" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D42" s="8" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="16">
-        <f t="shared" si="0"/>
-        <v>38</v>
-      </c>
-      <c r="B43" s="9"/>
-      <c r="C43" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="D43" s="8" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="16">
-        <f t="shared" si="0"/>
-        <v>39</v>
-      </c>
-      <c r="B44" s="9"/>
-      <c r="C44" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="D44" s="8" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="16">
-        <f t="shared" si="0"/>
+      <c r="B62" s="24"/>
+      <c r="C62" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="D62" s="27"/>
+    </row>
+    <row r="63" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B63" s="24"/>
+      <c r="C63" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="D63" s="27"/>
+    </row>
+    <row r="64" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B64" s="24"/>
+      <c r="C64" s="27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D64" s="27"/>
+    </row>
+    <row r="65" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="B65" s="24"/>
+      <c r="C65" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="D65" s="27"/>
+    </row>
+    <row r="66" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66">
+        <f t="shared" si="0"/>
+        <v>61</v>
+      </c>
+      <c r="B66" s="24"/>
+      <c r="C66" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="D66" s="27"/>
+    </row>
+    <row r="67" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B67" s="24"/>
+      <c r="C67" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="D67" s="27"/>
+    </row>
+    <row r="68" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68">
+        <f t="shared" si="0"/>
+        <v>63</v>
+      </c>
+      <c r="B68" s="24"/>
+      <c r="C68" s="27" t="s">
+        <v>208</v>
+      </c>
+      <c r="D68" s="27"/>
+    </row>
+    <row r="69" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69">
+        <f t="shared" si="0"/>
+        <v>64</v>
+      </c>
+      <c r="B69" s="24"/>
+      <c r="C69" s="27" t="s">
+        <v>215</v>
+      </c>
+      <c r="D69" s="27"/>
+    </row>
+    <row r="70" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="B70" s="24"/>
+      <c r="C70" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="D70" s="27"/>
+    </row>
+    <row r="71" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71">
+        <f t="shared" si="0"/>
+        <v>66</v>
+      </c>
+      <c r="B71" s="24"/>
+      <c r="C71" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="D71" s="27"/>
+    </row>
+    <row r="72" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72">
+        <f t="shared" ref="A72:A118" si="1">A71+1</f>
+        <v>67</v>
+      </c>
+      <c r="B72" s="24"/>
+      <c r="C72" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="D72" s="27"/>
+    </row>
+    <row r="73" spans="1:4" s="23" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A73">
+        <f t="shared" si="1"/>
+        <v>68</v>
+      </c>
+      <c r="B73" s="24"/>
+      <c r="C73" s="27" t="s">
+        <v>217</v>
+      </c>
+      <c r="D73" s="27"/>
+    </row>
+    <row r="74" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A74">
+        <f t="shared" si="1"/>
+        <v>69</v>
+      </c>
+      <c r="B74" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="C74" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="D74" s="49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A75">
+        <f t="shared" si="1"/>
+        <v>70</v>
+      </c>
+      <c r="B75" s="9"/>
+      <c r="C75" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D75" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76">
+        <f t="shared" si="1"/>
+        <v>71</v>
+      </c>
+      <c r="B76" s="9"/>
+      <c r="C76" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D76" s="8" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77">
+        <f t="shared" si="1"/>
+        <v>72</v>
+      </c>
+      <c r="B77" s="9"/>
+      <c r="C77" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B45" s="7" t="s">
+      <c r="D77" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78">
+        <f t="shared" si="1"/>
         <v>73</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D45" s="8" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A46" s="16">
-        <f t="shared" si="0"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B46" s="9"/>
-      <c r="C46" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D46" s="8" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A47" s="16">
-        <f t="shared" si="0"/>
+      <c r="D78" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79">
+        <f t="shared" si="1"/>
+        <v>74</v>
+      </c>
+      <c r="B79" s="9"/>
+      <c r="C79" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="9"/>
-      <c r="C47" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="D47" s="8" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A48" s="16">
-        <f t="shared" si="0"/>
+      <c r="D79" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80">
+        <f t="shared" si="1"/>
+        <v>75</v>
+      </c>
+      <c r="B80" s="9"/>
+      <c r="C80" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B48" s="13"/>
-      <c r="C48" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D48" s="15" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A49" s="16">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B49" s="13"/>
-      <c r="C49" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="D49" s="15" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A50" s="16">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B50" s="13"/>
-      <c r="C50" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="16">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B51" s="9"/>
-      <c r="C51" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="D51" s="8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A52" s="16">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B52" s="9"/>
-      <c r="C52" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D52" s="8" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="16">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B53" s="9"/>
-      <c r="C53" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D53" s="8"/>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="16">
-        <f t="shared" si="0"/>
-        <v>49</v>
-      </c>
-      <c r="B54" s="9"/>
-      <c r="C54" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="16">
-        <f t="shared" si="0"/>
-        <v>50</v>
-      </c>
-      <c r="B55" s="9"/>
-      <c r="C55" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D55" s="8" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="16">
-        <f t="shared" si="0"/>
-        <v>51</v>
-      </c>
-      <c r="B56" s="9"/>
-      <c r="C56" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="D56" s="8"/>
-    </row>
-    <row r="57" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="16">
-        <f t="shared" si="0"/>
-        <v>52</v>
-      </c>
-      <c r="B57" s="9"/>
-      <c r="C57" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D57" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A58" s="16">
-        <f t="shared" si="0"/>
+      <c r="D80" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="B58" s="9"/>
-      <c r="C58" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D58" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A59" s="16">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B59" s="9"/>
-      <c r="C59" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="D59" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A60" s="16">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B60" s="9"/>
-      <c r="C60" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="D60" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="16">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B61" s="9"/>
-      <c r="C61" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="D61" s="8" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="16">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B62" s="9"/>
-      <c r="C62" s="3"/>
-      <c r="D62" s="8"/>
-    </row>
-    <row r="63" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="16">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B63" s="7" t="s">
-        <v>74</v>
-      </c>
-      <c r="C63" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D63" s="8" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="16">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B64" s="9"/>
-      <c r="C64" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="D64" s="8" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="16">
-        <f t="shared" si="0"/>
-        <v>60</v>
-      </c>
-      <c r="B65" s="10"/>
-      <c r="C65" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="D65" s="12" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" s="20" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="16">
-        <f t="shared" si="0"/>
-        <v>61</v>
-      </c>
-      <c r="B66" s="24"/>
-      <c r="C66" s="25" t="s">
-        <v>150</v>
-      </c>
-      <c r="D66" s="26" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="16">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B67" s="23" t="s">
-        <v>131</v>
-      </c>
-      <c r="C67" s="20" t="s">
-        <v>148</v>
-      </c>
-      <c r="D67" s="18" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="16">
-        <f t="shared" si="0"/>
-        <v>63</v>
-      </c>
-      <c r="B68" s="18"/>
-      <c r="C68" s="20" t="s">
-        <v>147</v>
-      </c>
-      <c r="D68" s="18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="16">
-        <f t="shared" si="0"/>
-        <v>64</v>
-      </c>
-      <c r="C69" s="18" t="s">
-        <v>135</v>
-      </c>
-      <c r="D69" s="18" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="16">
-        <f t="shared" si="0"/>
-        <v>65</v>
-      </c>
-      <c r="C70" s="18" t="s">
-        <v>136</v>
-      </c>
-      <c r="D70" s="18" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="16">
-        <f t="shared" si="0"/>
-        <v>66</v>
-      </c>
-      <c r="C71" s="18" t="s">
-        <v>137</v>
-      </c>
-      <c r="D71" s="18" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="16">
-        <f t="shared" si="0"/>
-        <v>67</v>
-      </c>
-      <c r="C72" s="18" t="s">
-        <v>138</v>
-      </c>
-      <c r="D72" s="18" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="16">
-        <f t="shared" si="0"/>
-        <v>68</v>
-      </c>
-      <c r="C73" s="18" t="s">
-        <v>139</v>
-      </c>
-      <c r="D73" s="18" t="s">
-        <v>145</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="16">
-        <f t="shared" si="0"/>
-        <v>69</v>
-      </c>
-      <c r="C74" s="18" t="s">
-        <v>140</v>
-      </c>
-      <c r="D74" s="18" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="16">
-        <f t="shared" si="0"/>
-        <v>70</v>
-      </c>
-      <c r="C75" s="18" t="s">
-        <v>156</v>
-      </c>
-      <c r="D75" s="18" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="16">
-        <f t="shared" si="0"/>
-        <v>71</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="16">
-        <f t="shared" si="0"/>
-        <v>72</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="16">
-        <f t="shared" si="0"/>
-        <v>73</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="16">
-        <f t="shared" si="0"/>
-        <v>74</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" s="16">
-        <f t="shared" ref="A80:A113" si="1">A79+1</f>
-        <v>75</v>
-      </c>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A81" s="16">
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81">
         <f t="shared" si="1"/>
         <v>76</v>
       </c>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A82" s="16">
+      <c r="B81" s="9"/>
+      <c r="C81" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="D81" s="8" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82">
         <f t="shared" si="1"/>
         <v>77</v>
       </c>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A83" s="16">
+      <c r="B82" s="9"/>
+      <c r="C82" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="D82" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83">
         <f t="shared" si="1"/>
         <v>78</v>
       </c>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A84" s="16">
+      <c r="B83" s="9"/>
+      <c r="C83" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D83" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84">
         <f t="shared" si="1"/>
         <v>79</v>
       </c>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A85" s="16">
+      <c r="B84" s="9"/>
+      <c r="C84" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D84" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85">
         <f t="shared" si="1"/>
         <v>80</v>
       </c>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A86" s="16">
+      <c r="B85" s="9"/>
+      <c r="C85" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="D85" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86">
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A87" s="16">
+      <c r="B86" s="9"/>
+      <c r="C86" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D86" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87">
         <f t="shared" si="1"/>
         <v>82</v>
       </c>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A88" s="16">
+      <c r="B87" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="C87" s="48" t="s">
+        <v>19</v>
+      </c>
+      <c r="D87" s="49" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A88">
         <f t="shared" si="1"/>
         <v>83</v>
       </c>
-    </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A89" s="16">
+      <c r="B88" s="9"/>
+      <c r="C88" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D88" s="8" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A89">
         <f t="shared" si="1"/>
         <v>84</v>
       </c>
-    </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A90" s="16">
+      <c r="B89" s="9"/>
+      <c r="C89" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="D89" s="8" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A90">
         <f t="shared" si="1"/>
         <v>85</v>
       </c>
-    </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A91" s="16">
+      <c r="B90" s="13"/>
+      <c r="C90" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A91">
         <f t="shared" si="1"/>
         <v>86</v>
       </c>
-    </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A92" s="16">
+      <c r="B91" s="13"/>
+      <c r="C91" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="D91" s="15" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A92">
         <f t="shared" si="1"/>
         <v>87</v>
       </c>
-    </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A93" s="16">
+      <c r="B92" s="13"/>
+      <c r="C92" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="D92" s="15" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A93">
         <f t="shared" si="1"/>
         <v>88</v>
       </c>
-    </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A94" s="16">
+      <c r="B93" s="9"/>
+      <c r="C93" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="D93" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+      <c r="A94">
         <f t="shared" si="1"/>
         <v>89</v>
       </c>
-    </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A95" s="16">
+      <c r="B94" s="9"/>
+      <c r="C94" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D94" s="8" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95">
         <f t="shared" si="1"/>
         <v>90</v>
       </c>
-    </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A96" s="16">
+      <c r="B95" s="9"/>
+      <c r="C95" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D95" s="8"/>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96">
         <f t="shared" si="1"/>
         <v>91</v>
       </c>
-    </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A97" s="16">
+      <c r="B96" s="9"/>
+      <c r="C96" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="D96" s="8"/>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97">
         <f t="shared" si="1"/>
         <v>92</v>
       </c>
-    </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A98" s="16">
+      <c r="B97" s="9"/>
+      <c r="C97" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D97" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98">
         <f t="shared" si="1"/>
         <v>93</v>
       </c>
-    </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A99" s="16">
+      <c r="B98" s="9"/>
+      <c r="C98" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D98" s="8"/>
+    </row>
+    <row r="99" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A99">
         <f t="shared" si="1"/>
         <v>94</v>
       </c>
-    </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A100" s="16">
+      <c r="B99" s="9"/>
+      <c r="C99" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="D99" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A100">
         <f t="shared" si="1"/>
         <v>95</v>
       </c>
-    </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A101" s="16">
+      <c r="B100" s="9"/>
+      <c r="C100" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D100" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A101">
         <f t="shared" si="1"/>
         <v>96</v>
       </c>
-    </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A102" s="16">
+      <c r="B101" s="9"/>
+      <c r="C101" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D101" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A102">
         <f t="shared" si="1"/>
         <v>97</v>
       </c>
-    </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A103" s="16">
+      <c r="B102" s="9"/>
+      <c r="C102" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D102" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="103" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A103">
         <f t="shared" si="1"/>
         <v>98</v>
       </c>
-    </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A104" s="16">
+      <c r="B103" s="9"/>
+      <c r="C103" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="D103" s="8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A104">
         <f t="shared" si="1"/>
         <v>99</v>
       </c>
-    </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A105" s="16">
+      <c r="B104" s="9"/>
+      <c r="C104" s="3"/>
+      <c r="D104" s="8"/>
+    </row>
+    <row r="105" spans="1:4" ht="29.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A105">
         <f t="shared" si="1"/>
         <v>100</v>
       </c>
-    </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A106" s="16">
+      <c r="B105" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="C105" s="48" t="s">
+        <v>74</v>
+      </c>
+      <c r="D105" s="49" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A106">
         <f t="shared" si="1"/>
         <v>101</v>
       </c>
-    </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A107" s="16">
+      <c r="B106" s="9"/>
+      <c r="C106" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D106" s="8" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="107" spans="1:4" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A107">
         <f t="shared" si="1"/>
         <v>102</v>
       </c>
-    </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A108" s="16">
+      <c r="B107" s="10"/>
+      <c r="C107" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="D107" s="12" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="108" spans="1:4" s="18" customFormat="1" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A108">
         <f t="shared" si="1"/>
         <v>103</v>
       </c>
-    </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A109" s="16">
+      <c r="B108" s="45"/>
+      <c r="C108" s="46" t="s">
+        <v>149</v>
+      </c>
+      <c r="D108" s="47" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A109">
         <f t="shared" si="1"/>
         <v>104</v>
       </c>
-    </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A110" s="16">
+      <c r="B109" s="51" t="s">
+        <v>130</v>
+      </c>
+      <c r="C109" s="52" t="s">
+        <v>147</v>
+      </c>
+      <c r="D109" s="53" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A110">
         <f t="shared" si="1"/>
         <v>105</v>
       </c>
-    </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A111" s="16">
+      <c r="B110" s="54"/>
+      <c r="C110" s="36" t="s">
+        <v>146</v>
+      </c>
+      <c r="D110" s="19" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A111">
         <f t="shared" si="1"/>
         <v>106</v>
       </c>
-    </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A112" s="16">
+      <c r="B111" s="9"/>
+      <c r="C111" s="31" t="s">
+        <v>136</v>
+      </c>
+      <c r="D111" s="19" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A112">
         <f t="shared" si="1"/>
         <v>107</v>
       </c>
-    </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A113" s="16">
+      <c r="B112" s="9"/>
+      <c r="C112" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="D112" s="19" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113">
         <f t="shared" si="1"/>
         <v>108</v>
       </c>
+      <c r="B113" s="9"/>
+      <c r="C113" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="D113" s="19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114">
+        <f t="shared" si="1"/>
+        <v>109</v>
+      </c>
+      <c r="B114" s="9"/>
+      <c r="C114" s="31" t="s">
+        <v>134</v>
+      </c>
+      <c r="D114" s="19" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A115">
+        <f t="shared" si="1"/>
+        <v>110</v>
+      </c>
+      <c r="B115" s="9"/>
+      <c r="C115" s="31" t="s">
+        <v>138</v>
+      </c>
+      <c r="D115" s="19" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A116">
+        <f t="shared" si="1"/>
+        <v>111</v>
+      </c>
+      <c r="B116" s="9"/>
+      <c r="C116" s="31" t="s">
+        <v>139</v>
+      </c>
+      <c r="D116" s="19" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A117">
+        <f t="shared" si="1"/>
+        <v>112</v>
+      </c>
+      <c r="B117" s="9"/>
+      <c r="C117" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="D117" s="19" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="118" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A118">
+        <f t="shared" si="1"/>
+        <v>113</v>
+      </c>
+      <c r="B118" s="10"/>
+      <c r="C118" s="11" t="s">
+        <v>251</v>
+      </c>
+      <c r="D118" s="12" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="16"/>
+      <c r="C119" s="17"/>
+      <c r="D119" s="17"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" s="16"/>
+      <c r="C120" s="17"/>
+      <c r="D120" s="17"/>
+    </row>
+    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" s="16"/>
+    </row>
+    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A122" s="16"/>
+    </row>
+    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A123" s="16"/>
+    </row>
+    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A124" s="16"/>
+    </row>
+    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A125" s="16"/>
+    </row>
+    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A126" s="16"/>
+    </row>
+    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A127" s="16"/>
+    </row>
+    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A128" s="16"/>
+    </row>
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A129" s="16"/>
+    </row>
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A130" s="16"/>
+    </row>
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A131" s="16"/>
+    </row>
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A132" s="16"/>
+    </row>
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A133" s="16"/>
+    </row>
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A134" s="16"/>
+    </row>
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A135" s="16"/>
+    </row>
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A136" s="16"/>
+    </row>
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A137" s="16"/>
+    </row>
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A138" s="16"/>
+    </row>
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A139" s="16"/>
+    </row>
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A140" s="16"/>
+    </row>
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A141" s="16"/>
+    </row>
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A142" s="16"/>
+    </row>
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A143" s="16"/>
+    </row>
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A144" s="16"/>
+    </row>
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A145" s="16"/>
+    </row>
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A146" s="16"/>
+    </row>
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A147" s="16"/>
+    </row>
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A148" s="16"/>
+    </row>
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A149" s="16"/>
+    </row>
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A150" s="16"/>
+    </row>
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A151" s="16"/>
+    </row>
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A152" s="16"/>
+    </row>
+    <row r="153" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A153" s="16"/>
+    </row>
+    <row r="154" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A154" s="16"/>
+    </row>
+    <row r="155" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A155" s="16"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B3:D3"/>
+    <mergeCell ref="B1:D1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -3993,253 +4485,253 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="50.85546875" customWidth="1"/>
-    <col min="3" max="3" width="53.28515625" customWidth="1"/>
+    <col min="2" max="2" width="51.7109375" customWidth="1"/>
+    <col min="3" max="3" width="63.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="27" t="s">
+      <c r="A1" s="20" t="s">
+        <v>165</v>
+      </c>
+      <c r="B1" s="20" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="C1" s="20" t="s">
         <v>167</v>
       </c>
-      <c r="C1" s="27" t="s">
-        <v>168</v>
-      </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="27">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="17" t="s">
-        <v>112</v>
+      <c r="B2" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="32" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="27">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="C3" t="s">
-        <v>111</v>
-      </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="27">
         <f t="shared" ref="A4:A20" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="27" t="s">
+        <v>112</v>
+      </c>
+      <c r="C4" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="27">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>114</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5">
-        <f t="shared" si="0"/>
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="C5" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C5" t="s">
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="27">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="B6" s="27" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <f t="shared" si="0"/>
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+      <c r="C6" s="27" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="27">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="B7" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C7" s="27" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="27">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="27">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>121</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="27">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="B10" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="C10" s="27" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="27">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>125</v>
+      </c>
+      <c r="C11" s="34" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
+      <c r="A12" s="27">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="B12" s="35" t="s">
         <v>128</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7">
-        <f t="shared" si="0"/>
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>118</v>
-      </c>
-      <c r="C7" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8">
-        <f t="shared" si="0"/>
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>120</v>
-      </c>
-      <c r="C8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9">
-        <f t="shared" si="0"/>
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>122</v>
-      </c>
-      <c r="C9" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10">
-        <f t="shared" si="0"/>
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>124</v>
-      </c>
-      <c r="C10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>126</v>
-      </c>
-      <c r="C11" s="19" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" ht="60" x14ac:dyDescent="0.25">
-      <c r="A12">
-        <f t="shared" si="0"/>
-        <v>11</v>
-      </c>
-      <c r="B12" s="21" t="s">
+      <c r="C12" s="34" t="s">
         <v>129</v>
       </c>
-      <c r="C12" s="19" t="s">
-        <v>130</v>
-      </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13">
+      <c r="A13" s="27">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="33" t="s">
+        <v>132</v>
+      </c>
+      <c r="C13" s="34" t="s">
         <v>133</v>
       </c>
-      <c r="C13" s="19" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14">
+    </row>
+    <row r="14" spans="1:3" s="18" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="27">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B14" s="20" t="s">
+      <c r="B14" s="36" t="s">
+        <v>151</v>
+      </c>
+      <c r="C14" s="36" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" s="18" customFormat="1" ht="75" x14ac:dyDescent="0.25">
+      <c r="A15" s="27">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="B15" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="C14" s="20" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" s="20" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <f t="shared" si="0"/>
-        <v>14</v>
-      </c>
-      <c r="B15" s="21" t="s">
+      <c r="C15" s="34" t="s">
         <v>153</v>
       </c>
-      <c r="C15" s="19" t="s">
-        <v>154</v>
-      </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16">
+      <c r="A16" s="27">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B16" s="21" t="s">
+      <c r="B16" s="35" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="C16" s="21" t="s">
+    </row>
+    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
+      <c r="A17" s="27">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B17" s="35" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" ht="75" x14ac:dyDescent="0.25">
-      <c r="A17">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B17" s="21" t="s">
+      <c r="C17" s="33" t="s">
         <v>164</v>
       </c>
-      <c r="C17" s="22" t="s">
-        <v>165</v>
-      </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18">
+      <c r="A18" s="27">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B18" s="21" t="s">
+      <c r="B18" s="35" t="s">
+        <v>241</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="27">
+        <f t="shared" si="0"/>
+        <v>18</v>
+      </c>
+      <c r="B19" s="35" t="s">
+        <v>240</v>
+      </c>
+      <c r="C19" s="27" t="s">
         <v>245</v>
       </c>
-      <c r="C18" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19">
-        <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="B19" s="21" t="s">
-        <v>244</v>
-      </c>
-      <c r="C19" t="s">
-        <v>249</v>
-      </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20">
+      <c r="A20" s="27">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B20" s="21" t="s">
-        <v>246</v>
-      </c>
-      <c r="C20" t="s">
-        <v>247</v>
+      <c r="B20" s="35" t="s">
+        <v>242</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>243</v>
       </c>
     </row>
   </sheetData>

</xml_diff>